<commit_message>
parameter for phantom and pad renamed network communication reenabled
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="107">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">-Inf</t>
+    <t xml:space="preserve">-inf</t>
   </si>
   <si>
     <t xml:space="preserve">KickOut</t>
@@ -112,10 +112,10 @@
     <t xml:space="preserve">BassDI</t>
   </si>
   <si>
+    <t xml:space="preserve">BassMi</t>
+  </si>
+  <si>
     <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BassMi</t>
   </si>
   <si>
     <t xml:space="preserve">EGit1L</t>
@@ -433,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,6 +476,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1272,7 +1276,7 @@
   <dimension ref="A1:XFD131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1701,7 +1705,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
@@ -1722,10 +1726,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
@@ -4411,6 +4415,16 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E129" type="list">
+      <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-inf"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C129" type="list">
+      <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4429,7 +4443,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4471,24 +4485,6 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5584,7 +5580,7 @@
   <dimension ref="A1:Z129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6130,7 +6126,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <f aca="false">[1]Channels!A38</f>
         <v>37</v>
@@ -6140,7 +6136,7 @@
         <v>Divrs1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <f aca="false">[1]Channels!A39</f>
         <v>38</v>
@@ -6150,7 +6146,7 @@
         <v>Divrs2</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <f aca="false">[1]Channels!A40</f>
         <v>39</v>
@@ -6160,7 +6156,7 @@
         <v>Divrs3</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <f aca="false">[1]Channels!A41</f>
         <v>40</v>
@@ -6274,7 +6270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <f aca="false">[1]Channels!A50</f>
         <v>49</v>
@@ -6284,7 +6280,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <f aca="false">[1]Channels!A51</f>
         <v>50</v>
@@ -6294,7 +6290,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <f aca="false">[1]Channels!A52</f>
         <v>51</v>
@@ -6304,7 +6300,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
         <f aca="false">[1]Channels!A53</f>
         <v>52</v>
@@ -6314,7 +6310,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
         <f aca="false">[1]Channels!A54</f>
         <v>53</v>
@@ -6324,7 +6320,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <f aca="false">[1]Channels!A55</f>
         <v>54</v>
@@ -6334,7 +6330,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
         <f aca="false">[1]Channels!A56</f>
         <v>55</v>
@@ -6344,7 +6340,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
         <f aca="false">[1]Channels!A57</f>
         <v>56</v>
@@ -6354,7 +6350,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <f aca="false">[1]Channels!A58</f>
         <v>57</v>
@@ -6364,7 +6360,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
         <f aca="false">[1]Channels!A59</f>
         <v>58</v>
@@ -6374,7 +6370,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
         <f aca="false">[1]Channels!A60</f>
         <v>59</v>
@@ -6384,7 +6380,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <f aca="false">[1]Channels!A61</f>
         <v>60</v>
@@ -6394,7 +6390,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
         <f aca="false">[1]Channels!A62</f>
         <v>61</v>
@@ -6404,7 +6400,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
         <f aca="false">[1]Channels!A63</f>
         <v>62</v>
@@ -6414,7 +6410,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <f aca="false">[1]Channels!A64</f>
         <v>63</v>
@@ -6424,7 +6420,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
         <f aca="false">[1]Channels!A65</f>
         <v>64</v>
@@ -6434,7 +6430,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <f aca="false">[1]Channels!A66</f>
         <v>65</v>
@@ -6444,7 +6440,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <f aca="false">[1]Channels!A67</f>
         <v>66</v>
@@ -6454,7 +6450,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <f aca="false">[1]Channels!A68</f>
         <v>67</v>
@@ -6464,7 +6460,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <f aca="false">[1]Channels!A69</f>
         <v>68</v>
@@ -6474,7 +6470,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
         <f aca="false">[1]Channels!A70</f>
         <v>69</v>
@@ -6484,7 +6480,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
         <f aca="false">[1]Channels!A71</f>
         <v>70</v>
@@ -6494,7 +6490,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
         <f aca="false">[1]Channels!A72</f>
         <v>71</v>
@@ -6504,7 +6500,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
         <f aca="false">[1]Channels!A73</f>
         <v>72</v>
@@ -6514,7 +6510,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
         <f aca="false">[1]Channels!A74</f>
         <v>73</v>
@@ -6524,7 +6520,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
         <f aca="false">[1]Channels!A75</f>
         <v>74</v>
@@ -6534,7 +6530,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
         <f aca="false">[1]Channels!A76</f>
         <v>75</v>
@@ -6544,7 +6540,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
         <f aca="false">[1]Channels!A77</f>
         <v>76</v>
@@ -6554,7 +6550,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
         <f aca="false">[1]Channels!A78</f>
         <v>77</v>
@@ -6564,7 +6560,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <f aca="false">[1]Channels!A79</f>
         <v>78</v>
@@ -6574,7 +6570,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
         <f aca="false">[1]Channels!A80</f>
         <v>79</v>
@@ -6584,7 +6580,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
         <f aca="false">[1]Channels!A81</f>
         <v>80</v>
@@ -6594,7 +6590,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
         <f aca="false">[1]Channels!A82</f>
         <v>81</v>
@@ -6604,7 +6600,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
         <f aca="false">[1]Channels!A83</f>
         <v>82</v>
@@ -6614,7 +6610,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
         <f aca="false">[1]Channels!A84</f>
         <v>83</v>
@@ -6624,7 +6620,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
         <f aca="false">[1]Channels!A85</f>
         <v>84</v>
@@ -6634,7 +6630,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
         <f aca="false">[1]Channels!A86</f>
         <v>85</v>
@@ -6644,7 +6640,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
         <f aca="false">[1]Channels!A87</f>
         <v>86</v>
@@ -6654,7 +6650,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
         <f aca="false">[1]Channels!A88</f>
         <v>87</v>
@@ -6664,7 +6660,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
         <f aca="false">[1]Channels!A89</f>
         <v>88</v>
@@ -6674,7 +6670,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
         <f aca="false">[1]Channels!A90</f>
         <v>89</v>
@@ -6684,7 +6680,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
         <f aca="false">[1]Channels!A91</f>
         <v>90</v>
@@ -6694,7 +6690,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
         <f aca="false">[1]Channels!A92</f>
         <v>91</v>
@@ -6704,7 +6700,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
         <f aca="false">[1]Channels!A93</f>
         <v>92</v>
@@ -6714,7 +6710,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
         <f aca="false">[1]Channels!A94</f>
         <v>93</v>
@@ -6724,7 +6720,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
         <f aca="false">[1]Channels!A95</f>
         <v>94</v>
@@ -6734,7 +6730,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
         <f aca="false">[1]Channels!A96</f>
         <v>95</v>
@@ -6744,7 +6740,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
         <f aca="false">[1]Channels!A97</f>
         <v>96</v>
@@ -6754,7 +6750,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
         <f aca="false">[1]Channels!A98</f>
         <v>97</v>
@@ -6764,7 +6760,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
         <f aca="false">[1]Channels!A99</f>
         <v>98</v>
@@ -6774,7 +6770,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
         <f aca="false">[1]Channels!A100</f>
         <v>99</v>
@@ -6784,7 +6780,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
         <f aca="false">[1]Channels!A101</f>
         <v>100</v>
@@ -6794,7 +6790,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
         <f aca="false">[1]Channels!A102</f>
         <v>101</v>
@@ -6804,7 +6800,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="n">
         <f aca="false">[1]Channels!A103</f>
         <v>102</v>
@@ -6814,7 +6810,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="n">
         <f aca="false">[1]Channels!A104</f>
         <v>103</v>
@@ -6824,7 +6820,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="n">
         <f aca="false">[1]Channels!A105</f>
         <v>104</v>
@@ -6834,7 +6830,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="n">
         <f aca="false">[1]Channels!A106</f>
         <v>105</v>
@@ -6844,7 +6840,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="n">
         <f aca="false">[1]Channels!A107</f>
         <v>106</v>
@@ -6854,7 +6850,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="n">
         <f aca="false">[1]Channels!A108</f>
         <v>107</v>
@@ -6864,7 +6860,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="n">
         <f aca="false">[1]Channels!A109</f>
         <v>108</v>
@@ -6874,7 +6870,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="n">
         <f aca="false">[1]Channels!A110</f>
         <v>109</v>
@@ -6884,7 +6880,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="n">
         <f aca="false">[1]Channels!A111</f>
         <v>110</v>
@@ -6894,7 +6890,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="n">
         <f aca="false">[1]Channels!A112</f>
         <v>111</v>
@@ -6904,7 +6900,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="n">
         <f aca="false">[1]Channels!A113</f>
         <v>112</v>
@@ -6914,7 +6910,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="n">
         <f aca="false">[1]Channels!A114</f>
         <v>113</v>
@@ -6924,7 +6920,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="n">
         <f aca="false">[1]Channels!A115</f>
         <v>114</v>
@@ -6934,7 +6930,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="n">
         <f aca="false">[1]Channels!A116</f>
         <v>115</v>
@@ -6944,7 +6940,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="n">
         <f aca="false">[1]Channels!A117</f>
         <v>116</v>
@@ -6954,7 +6950,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="n">
         <f aca="false">[1]Channels!A118</f>
         <v>117</v>
@@ -6964,7 +6960,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="n">
         <f aca="false">[1]Channels!A119</f>
         <v>118</v>
@@ -6974,7 +6970,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="n">
         <f aca="false">[1]Channels!A120</f>
         <v>119</v>
@@ -6984,7 +6980,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="n">
         <f aca="false">[1]Channels!A121</f>
         <v>120</v>
@@ -6994,7 +6990,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="n">
         <f aca="false">[1]Channels!A122</f>
         <v>121</v>
@@ -7004,7 +7000,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="n">
         <f aca="false">[1]Channels!A123</f>
         <v>122</v>
@@ -7014,7 +7010,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="n">
         <f aca="false">[1]Channels!A124</f>
         <v>123</v>
@@ -7024,7 +7020,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="n">
         <f aca="false">[1]Channels!A125</f>
         <v>124</v>
@@ -7034,7 +7030,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="n">
         <f aca="false">[1]Channels!A126</f>
         <v>125</v>
@@ -7044,7 +7040,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="n">
         <f aca="false">[1]Channels!A127</f>
         <v>126</v>
@@ -7054,7 +7050,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="n">
         <f aca="false">[1]Channels!A128</f>
         <v>127</v>
@@ -7064,7 +7060,7 @@
         <v>empty</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="n">
         <f aca="false">[1]Channels!A129</f>
         <v>128</v>
@@ -7090,10 +7086,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7103,7 +7099,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="57.46"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -7114,7 +7110,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -7125,6 +7121,13 @@
         <v>106</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Reaper Session Creator added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="107">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">(C)DM48 End</t>
   </si>
   <si>
-    <t xml:space="preserve">(C)DM64</t>
+    <t xml:space="preserve">(C)DM64 End</t>
   </si>
   <si>
     <t xml:space="preserve">DCA1</t>
@@ -391,12 +391,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE994"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEDCE6"/>
+        <bgColor rgb="FFC6D9F1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -470,16 +482,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -566,7 +578,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEDCE6"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -582,7 +594,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFE994"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -1276,7 +1288,7 @@
   <dimension ref="A1:XFD131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4392,7 +4404,7 @@
       <c r="A131" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576 H1:H1048576">
+  <conditionalFormatting sqref="H1:H1048576 C1:C1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>
@@ -4443,7 +4455,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4472,19 +4484,37 @@
       <c r="E1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5597,76 +5627,76 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="11" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reaper folder generation right next to individual inputfile
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="85">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -207,9 +207,9 @@
     <t xml:space="preserve">BV4</t>
   </si>
   <si>
-    <t xml:space="preserve">Indication End Channel
+    <t xml:space="preserve">Indication Start/End Channel
 For
-Mixrack / Extenders 
+Mixrack / Expanders
 </t>
   </si>
   <si>
@@ -234,16 +234,73 @@
     <t xml:space="preserve">DX3 Pad</t>
   </si>
   <si>
+    <t xml:space="preserve">Slink Phantom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slink Pad</t>
+  </si>
+  <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
+    <t xml:space="preserve">Avantis Surface</t>
+  </si>
+  <si>
     <t xml:space="preserve">(C)DM32 End +  DX1/3 End</t>
   </si>
   <si>
-    <t xml:space="preserve">(C)DM48 End</t>
+    <t xml:space="preserve">(C)DM48 End + GX4816</t>
   </si>
   <si>
     <t xml:space="preserve">(C)DM64 End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slink-DX1 Start</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Slink-DX1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> End</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Slink-DX2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Start</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Slink-DX2 End</t>
   </si>
   <si>
     <t xml:space="preserve">Property</t>
@@ -268,7 +325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -299,8 +356,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +380,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDEDCE6"/>
         <bgColor rgb="FFC6D9F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
   </fills>
@@ -354,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,6 +466,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -478,7 +555,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
@@ -532,8 +609,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="J2:J129 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2534,10 +2611,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2548,9 +2625,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="3.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="3.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="3.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="74.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -2574,6 +2652,12 @@
       </c>
       <c r="H1" s="10" t="s">
         <v>68</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2581,22 +2665,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,22 +2694,28 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,22 +2723,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,22 +2752,28 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,22 +2781,28 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,22 +2810,28 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,22 +2839,28 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,22 +2868,28 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,22 +2897,28 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,22 +2926,28 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,45 +2955,60 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2857,22 +3016,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,22 +3045,28 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,22 +3074,28 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,22 +3103,28 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,22 +3132,28 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2972,22 +3161,28 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,22 +3190,28 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,22 +3219,28 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3041,22 +3248,28 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,22 +3277,28 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,22 +3306,28 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,22 +3335,28 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,22 +3364,28 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,22 +3393,28 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3179,22 +3422,28 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,22 +3451,28 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,22 +3480,28 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,22 +3509,28 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3271,48 +3538,60 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,10 +3599,16 @@
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,10 +3616,16 @@
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,10 +3633,16 @@
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3353,10 +3650,16 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3364,10 +3667,16 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,10 +3684,16 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,10 +3701,16 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3397,10 +3718,16 @@
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3408,10 +3735,16 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3419,10 +3752,16 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,10 +3769,16 @@
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3441,10 +3786,16 @@
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,10 +3803,16 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,10 +3820,16 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,24 +3837,36 @@
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,10 +3874,16 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3510,10 +3891,16 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,10 +3908,16 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3532,10 +3925,16 @@
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3543,10 +3942,16 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,10 +3959,16 @@
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,10 +3976,16 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3576,10 +3993,16 @@
         <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3587,10 +4010,16 @@
         <v>57</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3598,10 +4027,16 @@
         <v>58</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,10 +4044,16 @@
         <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3620,10 +4061,16 @@
         <v>60</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,10 +4078,16 @@
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3642,10 +4095,16 @@
         <v>62</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3653,24 +4112,752 @@
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>69</v>
+      <c r="I70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="2" t="n">
+        <v>82</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J84" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="2" t="n">
+        <v>84</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J86" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="2" t="n">
+        <v>86</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J87" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J89" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J90" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="I93" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J93" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J94" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="I95" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J95" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J96" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="I97" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J97" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="I98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J98" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="I99" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J99" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="I100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J100" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I101" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J101" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="I102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J102" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="I103" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J103" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="I104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J104" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="I105" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J105" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="I106" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J106" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="I107" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J107" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="I108" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J108" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="I109" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J109" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="I111" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J111" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="I112" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J112" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="I113" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J113" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="I114" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J114" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="I115" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J115" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="I116" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J116" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="I117" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J117" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="I118" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J118" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="2" t="n">
+        <v>118</v>
+      </c>
+      <c r="I119" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J119" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="I120" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J120" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="I121" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J121" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="I122" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="I123" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J123" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="I124" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J124" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="I125" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J125" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="I126" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J126" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="I127" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J127" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="I128" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J128" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="I129" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J129" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3692,7 +4879,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="J2:J129 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3704,24 +4891,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
doc updated, template updated
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="87">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -393,7 +393,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,10 +403,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,8 +583,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H129"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,31 +592,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="XFA1" s="1"/>
@@ -632,19 +628,19 @@
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -652,19 +648,19 @@
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -672,19 +668,19 @@
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -692,19 +688,19 @@
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -712,19 +708,19 @@
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -732,19 +728,19 @@
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -752,19 +748,19 @@
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -772,19 +768,19 @@
       <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -792,19 +788,19 @@
       <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -812,19 +808,19 @@
       <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -832,19 +828,19 @@
       <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -852,19 +848,19 @@
       <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -872,19 +868,19 @@
       <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -892,19 +888,19 @@
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="G15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -912,19 +908,19 @@
       <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -932,19 +928,19 @@
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -952,19 +948,19 @@
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -972,19 +968,19 @@
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -992,19 +988,19 @@
       <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1012,19 +1008,19 @@
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1032,19 +1028,19 @@
       <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="G22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1052,19 +1048,19 @@
       <c r="A23" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="G23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1072,19 +1068,19 @@
       <c r="A24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="G24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1092,19 +1088,19 @@
       <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1112,19 +1108,19 @@
       <c r="A26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="G26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1132,19 +1128,19 @@
       <c r="A27" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="G27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1152,19 +1148,19 @@
       <c r="A28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="3" t="s">
+      <c r="G28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1172,19 +1168,19 @@
       <c r="A29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="G29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1192,19 +1188,19 @@
       <c r="A30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="G30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1212,19 +1208,19 @@
       <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="G31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1232,19 +1228,19 @@
       <c r="A32" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="3" t="s">
+      <c r="G32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1252,19 +1248,19 @@
       <c r="A33" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="3" t="s">
+      <c r="G33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1272,19 +1268,19 @@
       <c r="A34" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="3" t="s">
+      <c r="G34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1292,19 +1288,19 @@
       <c r="A35" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="G35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1312,19 +1308,19 @@
       <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="3" t="s">
+      <c r="G36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1332,19 +1328,19 @@
       <c r="A37" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="G37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1352,19 +1348,19 @@
       <c r="A38" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="3" t="s">
+      <c r="G38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1372,19 +1368,19 @@
       <c r="A39" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="3" t="s">
+      <c r="G39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1392,19 +1388,19 @@
       <c r="A40" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="3" t="s">
+      <c r="G40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1412,19 +1408,19 @@
       <c r="A41" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="3" t="s">
+      <c r="G41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1432,19 +1428,19 @@
       <c r="A42" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="3" t="s">
+      <c r="G42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1452,19 +1448,19 @@
       <c r="A43" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H43" s="3" t="s">
+      <c r="G43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1472,19 +1468,19 @@
       <c r="A44" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="G44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1492,19 +1488,19 @@
       <c r="A45" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="3" t="s">
+      <c r="G45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1512,19 +1508,19 @@
       <c r="A46" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46" s="3" t="s">
+      <c r="G46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1532,19 +1528,19 @@
       <c r="A47" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="G47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1552,19 +1548,19 @@
       <c r="A48" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="G48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1572,19 +1568,19 @@
       <c r="A49" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="G49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1595,18 +1591,13 @@
       <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
@@ -1615,18 +1606,13 @@
       <c r="B51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
@@ -1635,18 +1621,13 @@
       <c r="B52" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
@@ -1655,18 +1636,13 @@
       <c r="B53" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
@@ -1675,18 +1651,13 @@
       <c r="B54" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
@@ -1695,18 +1666,13 @@
       <c r="B55" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G55" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
@@ -1715,18 +1681,13 @@
       <c r="B56" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
@@ -1735,18 +1696,13 @@
       <c r="B57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
@@ -1755,18 +1711,13 @@
       <c r="B58" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
@@ -1775,18 +1726,13 @@
       <c r="B59" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
@@ -1795,18 +1741,13 @@
       <c r="B60" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
@@ -1815,18 +1756,13 @@
       <c r="B61" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
@@ -1835,18 +1771,13 @@
       <c r="B62" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
@@ -1855,18 +1786,13 @@
       <c r="B63" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
@@ -1875,18 +1801,13 @@
       <c r="B64" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
@@ -1895,18 +1816,13 @@
       <c r="B65" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G65" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
@@ -1915,18 +1831,13 @@
       <c r="B66" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
@@ -1935,18 +1846,13 @@
       <c r="B67" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G67" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
@@ -1955,18 +1861,13 @@
       <c r="B68" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G68" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
@@ -1975,18 +1876,13 @@
       <c r="B69" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
@@ -1995,18 +1891,13 @@
       <c r="B70" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G70" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
@@ -2015,18 +1906,13 @@
       <c r="B71" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G71" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
@@ -2035,18 +1921,13 @@
       <c r="B72" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
@@ -2055,18 +1936,13 @@
       <c r="B73" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G73" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
@@ -2075,18 +1951,13 @@
       <c r="B74" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
@@ -2095,18 +1966,13 @@
       <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G75" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
@@ -2115,18 +1981,13 @@
       <c r="B76" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G76" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
@@ -2135,18 +1996,13 @@
       <c r="B77" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G77" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
@@ -2155,18 +2011,13 @@
       <c r="B78" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
@@ -2175,18 +2026,13 @@
       <c r="B79" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -2195,18 +2041,13 @@
       <c r="B80" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G80" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
@@ -2215,18 +2056,13 @@
       <c r="B81" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G81" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
@@ -2235,18 +2071,13 @@
       <c r="B82" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G82" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
@@ -2255,18 +2086,13 @@
       <c r="B83" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G83" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
@@ -2275,18 +2101,13 @@
       <c r="B84" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G84" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
@@ -2295,18 +2116,13 @@
       <c r="B85" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G85" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
@@ -2315,18 +2131,13 @@
       <c r="B86" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G86" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
@@ -2335,18 +2146,13 @@
       <c r="B87" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G87" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
@@ -2355,18 +2161,13 @@
       <c r="B88" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G88" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
@@ -2375,18 +2176,13 @@
       <c r="B89" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G89" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
@@ -2395,18 +2191,13 @@
       <c r="B90" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G90" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -2415,18 +2206,13 @@
       <c r="B91" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G91" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
@@ -2435,18 +2221,13 @@
       <c r="B92" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G92" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
@@ -2455,18 +2236,13 @@
       <c r="B93" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G93" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
@@ -2475,18 +2251,13 @@
       <c r="B94" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
@@ -2495,18 +2266,13 @@
       <c r="B95" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G95" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
@@ -2515,18 +2281,13 @@
       <c r="B96" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G96" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
@@ -2535,18 +2296,13 @@
       <c r="B97" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C97" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G97" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
@@ -2555,18 +2311,13 @@
       <c r="B98" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G98" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
@@ -2575,18 +2326,13 @@
       <c r="B99" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C99" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G99" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
@@ -2595,18 +2341,13 @@
       <c r="B100" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G100" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
@@ -2615,18 +2356,13 @@
       <c r="B101" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G101" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
@@ -2635,18 +2371,13 @@
       <c r="B102" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C102" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G102" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="n">
@@ -2655,18 +2386,13 @@
       <c r="B103" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G103" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="n">
@@ -2675,18 +2401,13 @@
       <c r="B104" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G104" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="n">
@@ -2695,18 +2416,13 @@
       <c r="B105" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G105" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H105" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="n">
@@ -2715,18 +2431,13 @@
       <c r="B106" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C106" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G106" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="n">
@@ -2735,18 +2446,13 @@
       <c r="B107" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G107" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H107" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G107" s="6"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="n">
@@ -2755,18 +2461,13 @@
       <c r="B108" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C108" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G108" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G108" s="6"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="n">
@@ -2775,18 +2476,13 @@
       <c r="B109" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C109" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G109" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H109" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G109" s="6"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="n">
@@ -2795,18 +2491,13 @@
       <c r="B110" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C110" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G110" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H110" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G110" s="6"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="n">
@@ -2815,18 +2506,13 @@
       <c r="B111" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C111" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G111" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H111" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G111" s="6"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="n">
@@ -2835,18 +2521,13 @@
       <c r="B112" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C112" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G112" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G112" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="n">
@@ -2855,18 +2536,13 @@
       <c r="B113" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C113" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G113" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H113" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G113" s="6"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="n">
@@ -2875,18 +2551,13 @@
       <c r="B114" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C114" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G114" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G114" s="6"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="n">
@@ -2895,18 +2566,13 @@
       <c r="B115" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G115" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G115" s="6"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="n">
@@ -2915,18 +2581,13 @@
       <c r="B116" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G116" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G116" s="6"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="n">
@@ -2935,18 +2596,13 @@
       <c r="B117" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G117" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="n">
@@ -2955,18 +2611,13 @@
       <c r="B118" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G118" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G118" s="6"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="n">
@@ -2975,18 +2626,13 @@
       <c r="B119" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G119" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G119" s="6"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="n">
@@ -2995,18 +2641,13 @@
       <c r="B120" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C120" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G120" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="n">
@@ -3015,18 +2656,13 @@
       <c r="B121" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C121" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G121" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G121" s="6"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="n">
@@ -3035,18 +2671,13 @@
       <c r="B122" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C122" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G122" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G122" s="6"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="n">
@@ -3055,18 +2686,13 @@
       <c r="B123" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="C123" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G123" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H123" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G123" s="6"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="n">
@@ -3075,18 +2701,13 @@
       <c r="B124" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="C124" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G124" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G124" s="6"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="n">
@@ -3095,18 +2716,13 @@
       <c r="B125" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C125" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G125" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H125" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G125" s="6"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="n">
@@ -3115,18 +2731,13 @@
       <c r="B126" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C126" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G126" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H126" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G126" s="6"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="n">
@@ -3135,18 +2746,13 @@
       <c r="B127" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="C127" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G127" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H127" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G127" s="6"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="n">
@@ -3155,18 +2761,13 @@
       <c r="B128" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="C128" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G128" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H128" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G128" s="6"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="n">
@@ -3175,18 +2776,13 @@
       <c r="B129" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="7" t="s">
+      <c r="C129" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G129" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H129" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G129" s="6"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2"/>
@@ -3242,7 +2838,7 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="H2:H129 L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3257,37 +2853,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5109,7 +4705,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B96" s="2" t="n">
@@ -5123,7 +4719,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B97" s="2" t="n">
@@ -5478,7 +5074,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B129" s="2" t="n">
@@ -5510,7 +5106,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="H2:H129 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5521,21 +5117,21 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="6" t="n">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>

<commit_message>
doc updated constants introduced
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -583,8 +583,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
dcas, hpf_on, hpf_value, fader_level to model added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -693,8 +693,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,7 +725,7 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="XFC1" s="0"/>
+      <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
preliminary gain support added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="120">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t xml:space="preserve">DCA24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">Property</t>
@@ -681,7 +684,7 @@
   <dimension ref="A1:XFD131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>11</v>
@@ -777,7 +780,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>11</v>
@@ -806,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>11</v>
@@ -835,7 +838,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>11</v>
@@ -864,7 +867,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>11</v>
@@ -893,7 +896,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>11</v>
@@ -922,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>11</v>
@@ -951,7 +954,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>11</v>
@@ -980,7 +983,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>11</v>
@@ -1009,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>11</v>
@@ -1038,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>11</v>
@@ -1067,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>11</v>
@@ -1096,7 +1099,7 @@
         <v>11</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>11</v>
@@ -1125,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>11</v>
@@ -1154,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>11</v>
@@ -1183,7 +1186,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>11</v>
@@ -1212,7 +1215,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>11</v>
@@ -1241,7 +1244,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>11</v>
@@ -1270,7 +1273,7 @@
         <v>11</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>11</v>
@@ -1299,7 +1302,7 @@
         <v>11</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>11</v>
@@ -1328,7 +1331,7 @@
         <v>11</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>11</v>
@@ -1357,7 +1360,7 @@
         <v>11</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>11</v>
@@ -1386,7 +1389,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>11</v>
@@ -1415,7 +1418,7 @@
         <v>11</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>11</v>
@@ -1444,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>11</v>
@@ -1473,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>11</v>
@@ -1502,7 +1505,7 @@
         <v>11</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>11</v>
@@ -1531,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>11</v>
@@ -1560,7 +1563,7 @@
         <v>11</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>11</v>
@@ -1589,7 +1592,7 @@
         <v>11</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>11</v>
@@ -1618,7 +1621,7 @@
         <v>11</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>11</v>
@@ -1647,7 +1650,7 @@
         <v>11</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>11</v>
@@ -1676,7 +1679,7 @@
         <v>11</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>11</v>
@@ -1705,7 +1708,7 @@
         <v>11</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>11</v>
@@ -1734,7 +1737,7 @@
         <v>11</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>11</v>
@@ -1763,7 +1766,7 @@
         <v>11</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>11</v>
@@ -1792,7 +1795,7 @@
         <v>11</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>11</v>
@@ -1821,7 +1824,7 @@
         <v>11</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>11</v>
@@ -1850,7 +1853,7 @@
         <v>11</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>11</v>
@@ -1879,7 +1882,7 @@
         <v>11</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>11</v>
@@ -1908,7 +1911,7 @@
         <v>11</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>11</v>
@@ -1937,7 +1940,7 @@
         <v>11</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>11</v>
@@ -1966,7 +1969,7 @@
         <v>11</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>11</v>
@@ -1995,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>11</v>
@@ -2024,7 +2027,7 @@
         <v>11</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>11</v>
@@ -2053,7 +2056,7 @@
         <v>11</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>11</v>
@@ -2082,7 +2085,7 @@
         <v>11</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>11</v>
@@ -2111,7 +2114,7 @@
         <v>11</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>11</v>
@@ -2140,7 +2143,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I50" s="6"/>
     </row>
@@ -2164,7 +2167,7 @@
         <v>11</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I51" s="6"/>
     </row>
@@ -2188,7 +2191,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I52" s="6"/>
     </row>
@@ -2212,7 +2215,7 @@
         <v>11</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I53" s="6"/>
     </row>
@@ -2236,7 +2239,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I54" s="6"/>
     </row>
@@ -2260,7 +2263,7 @@
         <v>11</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I55" s="6"/>
     </row>
@@ -2284,7 +2287,7 @@
         <v>11</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I56" s="6"/>
     </row>
@@ -2308,7 +2311,7 @@
         <v>11</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I57" s="6"/>
     </row>
@@ -2332,7 +2335,7 @@
         <v>11</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I58" s="6"/>
     </row>
@@ -2356,7 +2359,7 @@
         <v>11</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I59" s="6"/>
     </row>
@@ -2380,7 +2383,7 @@
         <v>11</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I60" s="6"/>
     </row>
@@ -2404,7 +2407,7 @@
         <v>11</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I61" s="6"/>
     </row>
@@ -2428,7 +2431,7 @@
         <v>11</v>
       </c>
       <c r="G62" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I62" s="6"/>
     </row>
@@ -2452,7 +2455,7 @@
         <v>11</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I63" s="6"/>
     </row>
@@ -2476,7 +2479,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I64" s="6"/>
     </row>
@@ -2500,7 +2503,7 @@
         <v>11</v>
       </c>
       <c r="G65" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I65" s="6"/>
     </row>
@@ -2524,7 +2527,7 @@
         <v>11</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I66" s="6"/>
     </row>
@@ -2548,7 +2551,7 @@
         <v>11</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I67" s="6"/>
     </row>
@@ -2572,7 +2575,7 @@
         <v>11</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I68" s="6"/>
     </row>
@@ -2596,7 +2599,7 @@
         <v>11</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I69" s="6"/>
     </row>
@@ -2620,7 +2623,7 @@
         <v>11</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I70" s="6"/>
     </row>
@@ -2644,7 +2647,7 @@
         <v>11</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I71" s="6"/>
     </row>
@@ -2668,7 +2671,7 @@
         <v>11</v>
       </c>
       <c r="G72" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I72" s="6"/>
     </row>
@@ -2692,7 +2695,7 @@
         <v>11</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I73" s="6"/>
     </row>
@@ -2716,7 +2719,7 @@
         <v>11</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I74" s="6"/>
     </row>
@@ -2740,7 +2743,7 @@
         <v>11</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I75" s="6"/>
     </row>
@@ -2764,7 +2767,7 @@
         <v>11</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I76" s="6"/>
     </row>
@@ -2788,7 +2791,7 @@
         <v>11</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I77" s="6"/>
     </row>
@@ -2812,7 +2815,7 @@
         <v>11</v>
       </c>
       <c r="G78" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I78" s="6"/>
     </row>
@@ -2836,7 +2839,7 @@
         <v>11</v>
       </c>
       <c r="G79" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I79" s="6"/>
     </row>
@@ -2860,7 +2863,7 @@
         <v>11</v>
       </c>
       <c r="G80" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I80" s="6"/>
     </row>
@@ -2884,7 +2887,7 @@
         <v>11</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I81" s="6"/>
     </row>
@@ -2908,7 +2911,7 @@
         <v>11</v>
       </c>
       <c r="G82" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I82" s="6"/>
     </row>
@@ -2932,7 +2935,7 @@
         <v>11</v>
       </c>
       <c r="G83" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I83" s="6"/>
     </row>
@@ -2956,7 +2959,7 @@
         <v>11</v>
       </c>
       <c r="G84" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I84" s="6"/>
     </row>
@@ -2980,7 +2983,7 @@
         <v>11</v>
       </c>
       <c r="G85" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I85" s="6"/>
     </row>
@@ -3004,7 +3007,7 @@
         <v>11</v>
       </c>
       <c r="G86" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I86" s="6"/>
     </row>
@@ -3028,7 +3031,7 @@
         <v>11</v>
       </c>
       <c r="G87" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I87" s="6"/>
     </row>
@@ -3052,7 +3055,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I88" s="6"/>
     </row>
@@ -3076,7 +3079,7 @@
         <v>11</v>
       </c>
       <c r="G89" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I89" s="6"/>
     </row>
@@ -3100,7 +3103,7 @@
         <v>11</v>
       </c>
       <c r="G90" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I90" s="6"/>
     </row>
@@ -3124,7 +3127,7 @@
         <v>11</v>
       </c>
       <c r="G91" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I91" s="6"/>
     </row>
@@ -3148,7 +3151,7 @@
         <v>11</v>
       </c>
       <c r="G92" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I92" s="6"/>
     </row>
@@ -3172,7 +3175,7 @@
         <v>11</v>
       </c>
       <c r="G93" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I93" s="6"/>
     </row>
@@ -3196,7 +3199,7 @@
         <v>11</v>
       </c>
       <c r="G94" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I94" s="6"/>
     </row>
@@ -3220,7 +3223,7 @@
         <v>11</v>
       </c>
       <c r="G95" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I95" s="6"/>
     </row>
@@ -3244,7 +3247,7 @@
         <v>11</v>
       </c>
       <c r="G96" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I96" s="6"/>
     </row>
@@ -3268,7 +3271,7 @@
         <v>11</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I97" s="6"/>
     </row>
@@ -3292,7 +3295,7 @@
         <v>11</v>
       </c>
       <c r="G98" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I98" s="6"/>
     </row>
@@ -3316,7 +3319,7 @@
         <v>11</v>
       </c>
       <c r="G99" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I99" s="6"/>
     </row>
@@ -3340,7 +3343,7 @@
         <v>11</v>
       </c>
       <c r="G100" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I100" s="6"/>
     </row>
@@ -3364,7 +3367,7 @@
         <v>11</v>
       </c>
       <c r="G101" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I101" s="6"/>
     </row>
@@ -3388,7 +3391,7 @@
         <v>11</v>
       </c>
       <c r="G102" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I102" s="6"/>
     </row>
@@ -3412,7 +3415,7 @@
         <v>11</v>
       </c>
       <c r="G103" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I103" s="6"/>
     </row>
@@ -3436,7 +3439,7 @@
         <v>11</v>
       </c>
       <c r="G104" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I104" s="6"/>
     </row>
@@ -3460,7 +3463,7 @@
         <v>11</v>
       </c>
       <c r="G105" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I105" s="6"/>
     </row>
@@ -3484,7 +3487,7 @@
         <v>11</v>
       </c>
       <c r="G106" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I106" s="6"/>
     </row>
@@ -3508,7 +3511,7 @@
         <v>11</v>
       </c>
       <c r="G107" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I107" s="6"/>
     </row>
@@ -3532,7 +3535,7 @@
         <v>11</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I108" s="6"/>
     </row>
@@ -3556,7 +3559,7 @@
         <v>11</v>
       </c>
       <c r="G109" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I109" s="6"/>
     </row>
@@ -3580,7 +3583,7 @@
         <v>11</v>
       </c>
       <c r="G110" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I110" s="6"/>
     </row>
@@ -3604,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="G111" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I111" s="6"/>
     </row>
@@ -3628,7 +3631,7 @@
         <v>11</v>
       </c>
       <c r="G112" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I112" s="6"/>
     </row>
@@ -3652,7 +3655,7 @@
         <v>11</v>
       </c>
       <c r="G113" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I113" s="6"/>
     </row>
@@ -3676,7 +3679,7 @@
         <v>11</v>
       </c>
       <c r="G114" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I114" s="6"/>
     </row>
@@ -3700,7 +3703,7 @@
         <v>11</v>
       </c>
       <c r="G115" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I115" s="6"/>
     </row>
@@ -3724,7 +3727,7 @@
         <v>11</v>
       </c>
       <c r="G116" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I116" s="6"/>
     </row>
@@ -3748,7 +3751,7 @@
         <v>11</v>
       </c>
       <c r="G117" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I117" s="6"/>
     </row>
@@ -3772,7 +3775,7 @@
         <v>11</v>
       </c>
       <c r="G118" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I118" s="6"/>
     </row>
@@ -3796,7 +3799,7 @@
         <v>11</v>
       </c>
       <c r="G119" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I119" s="6"/>
     </row>
@@ -3820,7 +3823,7 @@
         <v>11</v>
       </c>
       <c r="G120" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I120" s="6"/>
     </row>
@@ -3844,7 +3847,7 @@
         <v>11</v>
       </c>
       <c r="G121" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I121" s="6"/>
     </row>
@@ -3868,7 +3871,7 @@
         <v>11</v>
       </c>
       <c r="G122" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I122" s="6"/>
     </row>
@@ -3892,7 +3895,7 @@
         <v>11</v>
       </c>
       <c r="G123" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I123" s="6"/>
     </row>
@@ -3916,7 +3919,7 @@
         <v>11</v>
       </c>
       <c r="G124" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I124" s="6"/>
     </row>
@@ -3940,7 +3943,7 @@
         <v>11</v>
       </c>
       <c r="G125" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I125" s="6"/>
     </row>
@@ -3964,7 +3967,7 @@
         <v>11</v>
       </c>
       <c r="G126" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I126" s="6"/>
     </row>
@@ -3988,7 +3991,7 @@
         <v>11</v>
       </c>
       <c r="G127" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I127" s="6"/>
     </row>
@@ -4012,7 +4015,7 @@
         <v>11</v>
       </c>
       <c r="G128" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I128" s="6"/>
     </row>
@@ -4036,7 +4039,7 @@
         <v>11</v>
       </c>
       <c r="G129" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I129" s="6"/>
     </row>
@@ -4070,7 +4073,7 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C129" type="list">
       <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
@@ -4078,6 +4081,10 @@
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E129" type="list">
       <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-inf"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G129" type="decimal">
+      <formula1>20</formula1>
+      <formula2>2000</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4098,7 +4105,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4170,8 +4177,8 @@
       <c r="D2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
+      <c r="E2" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>81</v>
@@ -4179,8 +4186,8 @@
       <c r="H2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>0</v>
+      <c r="I2" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>81</v>
@@ -4188,8 +4195,8 @@
       <c r="L2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="2" t="n">
-        <v>0</v>
+      <c r="M2" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>81</v>
@@ -4197,8 +4204,8 @@
       <c r="P2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>0</v>
+      <c r="Q2" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,8 +4218,8 @@
       <c r="D3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
+      <c r="E3" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -4220,8 +4227,8 @@
       <c r="H3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <v>0</v>
+      <c r="I3" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>81</v>
@@ -4229,8 +4236,8 @@
       <c r="L3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M3" s="2" t="n">
-        <v>0</v>
+      <c r="M3" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>81</v>
@@ -4238,8 +4245,8 @@
       <c r="P3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="2" t="n">
-        <v>0</v>
+      <c r="Q3" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4252,8 +4259,8 @@
       <c r="D4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
+      <c r="E4" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>81</v>
@@ -4261,8 +4268,8 @@
       <c r="H4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <v>0</v>
+      <c r="I4" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>81</v>
@@ -4270,8 +4277,8 @@
       <c r="L4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M4" s="2" t="n">
-        <v>0</v>
+      <c r="M4" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>81</v>
@@ -4279,8 +4286,8 @@
       <c r="P4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="2" t="n">
-        <v>0</v>
+      <c r="Q4" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4293,8 +4300,8 @@
       <c r="D5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
+      <c r="E5" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -4302,8 +4309,8 @@
       <c r="H5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
+      <c r="I5" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>81</v>
@@ -4311,8 +4318,8 @@
       <c r="L5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M5" s="2" t="n">
-        <v>0</v>
+      <c r="M5" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>81</v>
@@ -4320,8 +4327,8 @@
       <c r="P5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q5" s="2" t="n">
-        <v>0</v>
+      <c r="Q5" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,8 +4341,8 @@
       <c r="D6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
+      <c r="E6" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>81</v>
@@ -4343,8 +4350,8 @@
       <c r="H6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
+      <c r="I6" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>81</v>
@@ -4352,8 +4359,8 @@
       <c r="L6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="2" t="n">
-        <v>0</v>
+      <c r="M6" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>81</v>
@@ -4361,8 +4368,8 @@
       <c r="P6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q6" s="2" t="n">
-        <v>0</v>
+      <c r="Q6" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,8 +4382,8 @@
       <c r="D7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
+      <c r="E7" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>81</v>
@@ -4384,8 +4391,8 @@
       <c r="H7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="2" t="n">
-        <v>0</v>
+      <c r="I7" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>81</v>
@@ -4393,8 +4400,8 @@
       <c r="L7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M7" s="2" t="n">
-        <v>0</v>
+      <c r="M7" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>81</v>
@@ -4402,8 +4409,8 @@
       <c r="P7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q7" s="2" t="n">
-        <v>0</v>
+      <c r="Q7" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4416,8 +4423,8 @@
       <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>0</v>
+      <c r="E8" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>81</v>
@@ -4425,8 +4432,8 @@
       <c r="H8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <v>0</v>
+      <c r="I8" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>81</v>
@@ -4434,8 +4441,8 @@
       <c r="L8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M8" s="2" t="n">
-        <v>0</v>
+      <c r="M8" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>81</v>
@@ -4443,8 +4450,8 @@
       <c r="P8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q8" s="2" t="n">
-        <v>0</v>
+      <c r="Q8" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4457,8 +4464,8 @@
       <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
+      <c r="E9" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>81</v>
@@ -4466,8 +4473,8 @@
       <c r="H9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <v>0</v>
+      <c r="I9" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>81</v>
@@ -4475,8 +4482,8 @@
       <c r="L9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M9" s="2" t="n">
-        <v>0</v>
+      <c r="M9" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>81</v>
@@ -4484,8 +4491,8 @@
       <c r="P9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="2" t="n">
-        <v>0</v>
+      <c r="Q9" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,8 +4505,8 @@
       <c r="D10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
+      <c r="E10" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>81</v>
@@ -4507,8 +4514,8 @@
       <c r="H10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
+      <c r="I10" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>81</v>
@@ -4516,8 +4523,8 @@
       <c r="L10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="2" t="n">
-        <v>0</v>
+      <c r="M10" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>81</v>
@@ -4525,8 +4532,8 @@
       <c r="P10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q10" s="2" t="n">
-        <v>0</v>
+      <c r="Q10" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,8 +4546,8 @@
       <c r="D11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
+      <c r="E11" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>81</v>
@@ -4548,8 +4555,8 @@
       <c r="H11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <v>0</v>
+      <c r="I11" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>81</v>
@@ -4557,8 +4564,8 @@
       <c r="L11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M11" s="2" t="n">
-        <v>0</v>
+      <c r="M11" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>81</v>
@@ -4566,8 +4573,8 @@
       <c r="P11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q11" s="2" t="n">
-        <v>0</v>
+      <c r="Q11" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,8 +4587,8 @@
       <c r="D12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>0</v>
+      <c r="E12" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>81</v>
@@ -4589,8 +4596,8 @@
       <c r="H12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="2" t="n">
-        <v>0</v>
+      <c r="I12" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>81</v>
@@ -4598,8 +4605,8 @@
       <c r="L12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M12" s="2" t="n">
-        <v>0</v>
+      <c r="M12" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>81</v>
@@ -4607,8 +4614,8 @@
       <c r="P12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="2" t="n">
-        <v>0</v>
+      <c r="Q12" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,8 +4631,8 @@
       <c r="D13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>0</v>
+      <c r="E13" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>81</v>
@@ -4633,8 +4640,8 @@
       <c r="H13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <v>0</v>
+      <c r="I13" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>81</v>
@@ -4642,8 +4649,8 @@
       <c r="L13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M13" s="2" t="n">
-        <v>0</v>
+      <c r="M13" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>81</v>
@@ -4651,8 +4658,8 @@
       <c r="P13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q13" s="2" t="n">
-        <v>0</v>
+      <c r="Q13" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,8 +4672,8 @@
       <c r="D14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>0</v>
+      <c r="E14" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>81</v>
@@ -4674,8 +4681,8 @@
       <c r="H14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
+      <c r="I14" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>81</v>
@@ -4683,8 +4690,8 @@
       <c r="L14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M14" s="2" t="n">
-        <v>0</v>
+      <c r="M14" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>81</v>
@@ -4692,8 +4699,8 @@
       <c r="P14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q14" s="2" t="n">
-        <v>0</v>
+      <c r="Q14" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,8 +4713,8 @@
       <c r="D15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>0</v>
+      <c r="E15" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>81</v>
@@ -4715,8 +4722,8 @@
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <v>0</v>
+      <c r="I15" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>81</v>
@@ -4724,8 +4731,8 @@
       <c r="L15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="2" t="n">
-        <v>0</v>
+      <c r="M15" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>81</v>
@@ -4733,8 +4740,8 @@
       <c r="P15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q15" s="2" t="n">
-        <v>0</v>
+      <c r="Q15" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4747,8 +4754,8 @@
       <c r="D16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="2" t="n">
-        <v>0</v>
+      <c r="E16" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>81</v>
@@ -4756,8 +4763,8 @@
       <c r="H16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <v>0</v>
+      <c r="I16" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>81</v>
@@ -4765,8 +4772,8 @@
       <c r="L16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M16" s="2" t="n">
-        <v>0</v>
+      <c r="M16" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>81</v>
@@ -4774,8 +4781,8 @@
       <c r="P16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q16" s="2" t="n">
-        <v>0</v>
+      <c r="Q16" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4788,8 +4795,8 @@
       <c r="D17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>0</v>
+      <c r="E17" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>81</v>
@@ -4797,8 +4804,8 @@
       <c r="H17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <v>0</v>
+      <c r="I17" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>81</v>
@@ -4806,8 +4813,8 @@
       <c r="L17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M17" s="2" t="n">
-        <v>0</v>
+      <c r="M17" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>81</v>
@@ -4815,8 +4822,8 @@
       <c r="P17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q17" s="2" t="n">
-        <v>0</v>
+      <c r="Q17" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4829,8 +4836,8 @@
       <c r="D18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
+      <c r="E18" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>81</v>
@@ -4838,8 +4845,8 @@
       <c r="H18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <v>0</v>
+      <c r="I18" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>81</v>
@@ -4847,8 +4854,8 @@
       <c r="L18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M18" s="2" t="n">
-        <v>0</v>
+      <c r="M18" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O18" s="2" t="s">
         <v>81</v>
@@ -4856,8 +4863,8 @@
       <c r="P18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q18" s="2" t="n">
-        <v>0</v>
+      <c r="Q18" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4870,8 +4877,8 @@
       <c r="D19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>0</v>
+      <c r="E19" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>81</v>
@@ -4879,8 +4886,8 @@
       <c r="H19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <v>0</v>
+      <c r="I19" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>81</v>
@@ -4888,8 +4895,8 @@
       <c r="L19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="2" t="n">
-        <v>0</v>
+      <c r="M19" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>81</v>
@@ -4897,8 +4904,8 @@
       <c r="P19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q19" s="2" t="n">
-        <v>0</v>
+      <c r="Q19" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,8 +4918,8 @@
       <c r="D20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>0</v>
+      <c r="E20" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>81</v>
@@ -4920,8 +4927,8 @@
       <c r="H20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="2" t="n">
-        <v>0</v>
+      <c r="I20" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>81</v>
@@ -4929,8 +4936,8 @@
       <c r="L20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M20" s="2" t="n">
-        <v>0</v>
+      <c r="M20" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>81</v>
@@ -4938,8 +4945,8 @@
       <c r="P20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q20" s="2" t="n">
-        <v>0</v>
+      <c r="Q20" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4952,8 +4959,8 @@
       <c r="D21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="2" t="n">
-        <v>0</v>
+      <c r="E21" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>81</v>
@@ -4961,8 +4968,8 @@
       <c r="H21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="2" t="n">
-        <v>0</v>
+      <c r="I21" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>81</v>
@@ -4970,8 +4977,8 @@
       <c r="L21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M21" s="2" t="n">
-        <v>0</v>
+      <c r="M21" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>81</v>
@@ -4979,8 +4986,8 @@
       <c r="P21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q21" s="2" t="n">
-        <v>0</v>
+      <c r="Q21" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4993,8 +5000,8 @@
       <c r="D22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="2" t="n">
-        <v>0</v>
+      <c r="E22" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>81</v>
@@ -5002,8 +5009,8 @@
       <c r="H22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I22" s="2" t="n">
-        <v>0</v>
+      <c r="I22" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>81</v>
@@ -5011,8 +5018,8 @@
       <c r="L22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M22" s="2" t="n">
-        <v>0</v>
+      <c r="M22" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>81</v>
@@ -5020,8 +5027,8 @@
       <c r="P22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q22" s="2" t="n">
-        <v>0</v>
+      <c r="Q22" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,8 +5041,8 @@
       <c r="D23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="2" t="n">
-        <v>0</v>
+      <c r="E23" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>81</v>
@@ -5043,8 +5050,8 @@
       <c r="H23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="2" t="n">
-        <v>0</v>
+      <c r="I23" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>81</v>
@@ -5052,8 +5059,8 @@
       <c r="L23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M23" s="2" t="n">
-        <v>0</v>
+      <c r="M23" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>81</v>
@@ -5061,8 +5068,8 @@
       <c r="P23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q23" s="2" t="n">
-        <v>0</v>
+      <c r="Q23" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,8 +5082,8 @@
       <c r="D24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="2" t="n">
-        <v>0</v>
+      <c r="E24" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>81</v>
@@ -5084,8 +5091,8 @@
       <c r="H24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="2" t="n">
-        <v>0</v>
+      <c r="I24" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>81</v>
@@ -5093,8 +5100,8 @@
       <c r="L24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M24" s="2" t="n">
-        <v>0</v>
+      <c r="M24" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O24" s="2" t="s">
         <v>81</v>
@@ -5102,8 +5109,8 @@
       <c r="P24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q24" s="2" t="n">
-        <v>0</v>
+      <c r="Q24" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,8 +5123,8 @@
       <c r="D25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="2" t="n">
-        <v>0</v>
+      <c r="E25" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>81</v>
@@ -5125,8 +5132,8 @@
       <c r="H25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I25" s="2" t="n">
-        <v>0</v>
+      <c r="I25" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>81</v>
@@ -5134,8 +5141,8 @@
       <c r="L25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M25" s="2" t="n">
-        <v>0</v>
+      <c r="M25" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>81</v>
@@ -5143,8 +5150,8 @@
       <c r="P25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q25" s="2" t="n">
-        <v>0</v>
+      <c r="Q25" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5157,8 +5164,8 @@
       <c r="D26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="2" t="n">
-        <v>0</v>
+      <c r="E26" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>81</v>
@@ -5166,8 +5173,8 @@
       <c r="H26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="2" t="n">
-        <v>0</v>
+      <c r="I26" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>81</v>
@@ -5175,8 +5182,8 @@
       <c r="L26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M26" s="2" t="n">
-        <v>0</v>
+      <c r="M26" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>81</v>
@@ -5184,8 +5191,8 @@
       <c r="P26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q26" s="2" t="n">
-        <v>0</v>
+      <c r="Q26" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5198,8 +5205,8 @@
       <c r="D27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
+      <c r="E27" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>81</v>
@@ -5207,8 +5214,8 @@
       <c r="H27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="2" t="n">
-        <v>0</v>
+      <c r="I27" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>81</v>
@@ -5216,8 +5223,8 @@
       <c r="L27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="2" t="n">
-        <v>0</v>
+      <c r="M27" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>81</v>
@@ -5225,8 +5232,8 @@
       <c r="P27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q27" s="2" t="n">
-        <v>0</v>
+      <c r="Q27" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5239,8 +5246,8 @@
       <c r="D28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
+      <c r="E28" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>81</v>
@@ -5248,8 +5255,8 @@
       <c r="H28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I28" s="2" t="n">
-        <v>0</v>
+      <c r="I28" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -5257,8 +5264,8 @@
       <c r="L28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M28" s="2" t="n">
-        <v>0</v>
+      <c r="M28" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>81</v>
@@ -5266,8 +5273,8 @@
       <c r="P28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q28" s="2" t="n">
-        <v>0</v>
+      <c r="Q28" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5280,8 +5287,8 @@
       <c r="D29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="2" t="n">
-        <v>0</v>
+      <c r="E29" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>81</v>
@@ -5289,8 +5296,8 @@
       <c r="H29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="2" t="n">
-        <v>0</v>
+      <c r="I29" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>81</v>
@@ -5298,8 +5305,8 @@
       <c r="L29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M29" s="2" t="n">
-        <v>0</v>
+      <c r="M29" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>81</v>
@@ -5307,8 +5314,8 @@
       <c r="P29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q29" s="2" t="n">
-        <v>0</v>
+      <c r="Q29" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5321,8 +5328,8 @@
       <c r="D30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>0</v>
+      <c r="E30" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>81</v>
@@ -5330,8 +5337,8 @@
       <c r="H30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="2" t="n">
-        <v>0</v>
+      <c r="I30" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>81</v>
@@ -5339,8 +5346,8 @@
       <c r="L30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M30" s="2" t="n">
-        <v>0</v>
+      <c r="M30" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>81</v>
@@ -5348,8 +5355,8 @@
       <c r="P30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q30" s="2" t="n">
-        <v>0</v>
+      <c r="Q30" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,8 +5369,8 @@
       <c r="D31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>0</v>
+      <c r="E31" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>81</v>
@@ -5371,8 +5378,8 @@
       <c r="H31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="2" t="n">
-        <v>0</v>
+      <c r="I31" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>81</v>
@@ -5380,8 +5387,8 @@
       <c r="L31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M31" s="2" t="n">
-        <v>0</v>
+      <c r="M31" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>81</v>
@@ -5389,8 +5396,8 @@
       <c r="P31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q31" s="2" t="n">
-        <v>0</v>
+      <c r="Q31" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5403,8 +5410,8 @@
       <c r="D32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="2" t="n">
-        <v>0</v>
+      <c r="E32" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>81</v>
@@ -5412,8 +5419,8 @@
       <c r="H32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I32" s="2" t="n">
-        <v>0</v>
+      <c r="I32" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>81</v>
@@ -5421,8 +5428,8 @@
       <c r="L32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M32" s="2" t="n">
-        <v>0</v>
+      <c r="M32" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>81</v>
@@ -5430,8 +5437,8 @@
       <c r="P32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q32" s="2" t="n">
-        <v>0</v>
+      <c r="Q32" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5447,8 +5454,8 @@
       <c r="D33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="2" t="n">
-        <v>0</v>
+      <c r="E33" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>81</v>
@@ -5456,8 +5463,8 @@
       <c r="H33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="2" t="n">
-        <v>0</v>
+      <c r="I33" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>81</v>
@@ -5465,8 +5472,8 @@
       <c r="L33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M33" s="2" t="n">
-        <v>0</v>
+      <c r="M33" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>81</v>
@@ -5474,8 +5481,8 @@
       <c r="P33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q33" s="2" t="n">
-        <v>0</v>
+      <c r="Q33" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5488,8 +5495,8 @@
       <c r="D34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="2" t="n">
-        <v>0</v>
+      <c r="E34" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>81</v>
@@ -5497,8 +5504,8 @@
       <c r="P34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q34" s="2" t="n">
-        <v>0</v>
+      <c r="Q34" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5511,8 +5518,8 @@
       <c r="D35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>0</v>
+      <c r="E35" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>81</v>
@@ -5520,8 +5527,8 @@
       <c r="P35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q35" s="2" t="n">
-        <v>0</v>
+      <c r="Q35" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5534,8 +5541,8 @@
       <c r="D36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="2" t="n">
-        <v>0</v>
+      <c r="E36" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>81</v>
@@ -5543,8 +5550,8 @@
       <c r="P36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q36" s="2" t="n">
-        <v>0</v>
+      <c r="Q36" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5557,8 +5564,8 @@
       <c r="D37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="2" t="n">
-        <v>0</v>
+      <c r="E37" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O37" s="2" t="s">
         <v>81</v>
@@ -5566,8 +5573,8 @@
       <c r="P37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q37" s="2" t="n">
-        <v>0</v>
+      <c r="Q37" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5580,8 +5587,8 @@
       <c r="D38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>0</v>
+      <c r="E38" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O38" s="2" t="s">
         <v>81</v>
@@ -5589,8 +5596,8 @@
       <c r="P38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q38" s="2" t="n">
-        <v>0</v>
+      <c r="Q38" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,8 +5610,8 @@
       <c r="D39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>0</v>
+      <c r="E39" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O39" s="2" t="s">
         <v>81</v>
@@ -5612,8 +5619,8 @@
       <c r="P39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q39" s="2" t="n">
-        <v>0</v>
+      <c r="Q39" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5626,8 +5633,8 @@
       <c r="D40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="2" t="n">
-        <v>0</v>
+      <c r="E40" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>81</v>
@@ -5635,8 +5642,8 @@
       <c r="P40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q40" s="2" t="n">
-        <v>0</v>
+      <c r="Q40" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,8 +5656,8 @@
       <c r="D41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>0</v>
+      <c r="E41" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>81</v>
@@ -5658,8 +5665,8 @@
       <c r="P41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q41" s="2" t="n">
-        <v>0</v>
+      <c r="Q41" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5672,8 +5679,8 @@
       <c r="D42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="2" t="n">
-        <v>0</v>
+      <c r="E42" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>81</v>
@@ -5681,8 +5688,8 @@
       <c r="P42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q42" s="2" t="n">
-        <v>0</v>
+      <c r="Q42" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5695,8 +5702,8 @@
       <c r="D43" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="2" t="n">
-        <v>0</v>
+      <c r="E43" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>81</v>
@@ -5704,8 +5711,8 @@
       <c r="P43" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q43" s="2" t="n">
-        <v>0</v>
+      <c r="Q43" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5718,8 +5725,8 @@
       <c r="D44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="2" t="n">
-        <v>0</v>
+      <c r="E44" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>81</v>
@@ -5727,8 +5734,8 @@
       <c r="P44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q44" s="2" t="n">
-        <v>0</v>
+      <c r="Q44" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5741,8 +5748,8 @@
       <c r="D45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E45" s="2" t="n">
-        <v>0</v>
+      <c r="E45" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>81</v>
@@ -5750,8 +5757,8 @@
       <c r="P45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q45" s="2" t="n">
-        <v>0</v>
+      <c r="Q45" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5764,8 +5771,8 @@
       <c r="D46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="2" t="n">
-        <v>0</v>
+      <c r="E46" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>81</v>
@@ -5773,8 +5780,8 @@
       <c r="P46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q46" s="2" t="n">
-        <v>0</v>
+      <c r="Q46" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5787,8 +5794,8 @@
       <c r="D47" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="2" t="n">
-        <v>0</v>
+      <c r="E47" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>81</v>
@@ -5796,8 +5803,8 @@
       <c r="P47" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q47" s="2" t="n">
-        <v>0</v>
+      <c r="Q47" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5810,8 +5817,8 @@
       <c r="D48" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="2" t="n">
-        <v>0</v>
+      <c r="E48" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>81</v>
@@ -5819,8 +5826,8 @@
       <c r="P48" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q48" s="2" t="n">
-        <v>0</v>
+      <c r="Q48" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,8 +5843,8 @@
       <c r="D49" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="2" t="n">
-        <v>0</v>
+      <c r="E49" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>81</v>
@@ -5845,8 +5852,8 @@
       <c r="P49" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q49" s="2" t="n">
-        <v>0</v>
+      <c r="Q49" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,8 +5866,8 @@
       <c r="D50" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E50" s="2" t="n">
-        <v>0</v>
+      <c r="E50" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>81</v>
@@ -5868,8 +5875,8 @@
       <c r="P50" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q50" s="2" t="n">
-        <v>0</v>
+      <c r="Q50" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5882,8 +5889,8 @@
       <c r="D51" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="2" t="n">
-        <v>0</v>
+      <c r="E51" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>81</v>
@@ -5891,8 +5898,8 @@
       <c r="P51" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q51" s="2" t="n">
-        <v>0</v>
+      <c r="Q51" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,8 +5912,8 @@
       <c r="D52" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E52" s="2" t="n">
-        <v>0</v>
+      <c r="E52" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>81</v>
@@ -5914,8 +5921,8 @@
       <c r="P52" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q52" s="2" t="n">
-        <v>0</v>
+      <c r="Q52" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,8 +5935,8 @@
       <c r="D53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="2" t="n">
-        <v>0</v>
+      <c r="E53" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>81</v>
@@ -5937,8 +5944,8 @@
       <c r="P53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q53" s="2" t="n">
-        <v>0</v>
+      <c r="Q53" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,8 +5958,8 @@
       <c r="D54" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="2" t="n">
-        <v>0</v>
+      <c r="E54" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>81</v>
@@ -5960,8 +5967,8 @@
       <c r="P54" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q54" s="2" t="n">
-        <v>0</v>
+      <c r="Q54" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5974,8 +5981,8 @@
       <c r="D55" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="2" t="n">
-        <v>0</v>
+      <c r="E55" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>81</v>
@@ -5983,8 +5990,8 @@
       <c r="P55" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q55" s="2" t="n">
-        <v>0</v>
+      <c r="Q55" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5997,8 +6004,8 @@
       <c r="D56" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="2" t="n">
-        <v>0</v>
+      <c r="E56" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>81</v>
@@ -6006,8 +6013,8 @@
       <c r="P56" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q56" s="2" t="n">
-        <v>0</v>
+      <c r="Q56" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6020,8 +6027,8 @@
       <c r="D57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="2" t="n">
-        <v>0</v>
+      <c r="E57" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>81</v>
@@ -6029,8 +6036,8 @@
       <c r="P57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q57" s="2" t="n">
-        <v>0</v>
+      <c r="Q57" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,8 +6050,8 @@
       <c r="D58" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E58" s="2" t="n">
-        <v>0</v>
+      <c r="E58" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>81</v>
@@ -6052,8 +6059,8 @@
       <c r="P58" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q58" s="2" t="n">
-        <v>0</v>
+      <c r="Q58" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6066,8 +6073,8 @@
       <c r="D59" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E59" s="2" t="n">
-        <v>0</v>
+      <c r="E59" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>81</v>
@@ -6075,8 +6082,8 @@
       <c r="P59" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q59" s="2" t="n">
-        <v>0</v>
+      <c r="Q59" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6089,8 +6096,8 @@
       <c r="D60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E60" s="2" t="n">
-        <v>0</v>
+      <c r="E60" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>81</v>
@@ -6098,8 +6105,8 @@
       <c r="P60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q60" s="2" t="n">
-        <v>0</v>
+      <c r="Q60" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,8 +6119,8 @@
       <c r="D61" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="2" t="n">
-        <v>0</v>
+      <c r="E61" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>81</v>
@@ -6121,8 +6128,8 @@
       <c r="P61" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q61" s="2" t="n">
-        <v>0</v>
+      <c r="Q61" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6135,8 +6142,8 @@
       <c r="D62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E62" s="2" t="n">
-        <v>0</v>
+      <c r="E62" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>81</v>
@@ -6144,8 +6151,8 @@
       <c r="P62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q62" s="2" t="n">
-        <v>0</v>
+      <c r="Q62" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6158,8 +6165,8 @@
       <c r="D63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="2" t="n">
-        <v>0</v>
+      <c r="E63" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>81</v>
@@ -6167,8 +6174,8 @@
       <c r="P63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q63" s="2" t="n">
-        <v>0</v>
+      <c r="Q63" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6181,8 +6188,8 @@
       <c r="D64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="2" t="n">
-        <v>0</v>
+      <c r="E64" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>81</v>
@@ -6190,8 +6197,8 @@
       <c r="P64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q64" s="2" t="n">
-        <v>0</v>
+      <c r="Q64" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6207,8 +6214,8 @@
       <c r="D65" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E65" s="2" t="n">
-        <v>0</v>
+      <c r="E65" s="6" t="n">
+        <v>25</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>81</v>
@@ -6216,8 +6223,8 @@
       <c r="P65" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q65" s="2" t="n">
-        <v>0</v>
+      <c r="Q65" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6233,8 +6240,8 @@
       <c r="P66" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q66" s="2" t="n">
-        <v>0</v>
+      <c r="Q66" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6247,8 +6254,8 @@
       <c r="P67" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q67" s="2" t="n">
-        <v>0</v>
+      <c r="Q67" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6261,8 +6268,8 @@
       <c r="P68" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q68" s="2" t="n">
-        <v>0</v>
+      <c r="Q68" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6275,8 +6282,8 @@
       <c r="P69" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q69" s="2" t="n">
-        <v>0</v>
+      <c r="Q69" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6289,8 +6296,8 @@
       <c r="P70" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q70" s="2" t="n">
-        <v>0</v>
+      <c r="Q70" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6303,8 +6310,8 @@
       <c r="P71" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q71" s="2" t="n">
-        <v>0</v>
+      <c r="Q71" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6317,8 +6324,8 @@
       <c r="P72" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q72" s="2" t="n">
-        <v>0</v>
+      <c r="Q72" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6331,8 +6338,8 @@
       <c r="P73" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q73" s="2" t="n">
-        <v>0</v>
+      <c r="Q73" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6345,8 +6352,8 @@
       <c r="P74" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q74" s="2" t="n">
-        <v>0</v>
+      <c r="Q74" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6359,8 +6366,8 @@
       <c r="P75" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q75" s="2" t="n">
-        <v>0</v>
+      <c r="Q75" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6373,8 +6380,8 @@
       <c r="P76" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q76" s="2" t="n">
-        <v>0</v>
+      <c r="Q76" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6387,8 +6394,8 @@
       <c r="P77" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q77" s="2" t="n">
-        <v>0</v>
+      <c r="Q77" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6401,8 +6408,8 @@
       <c r="P78" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q78" s="2" t="n">
-        <v>0</v>
+      <c r="Q78" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6415,8 +6422,8 @@
       <c r="P79" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q79" s="2" t="n">
-        <v>0</v>
+      <c r="Q79" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6429,8 +6436,8 @@
       <c r="P80" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q80" s="2" t="n">
-        <v>0</v>
+      <c r="Q80" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6443,8 +6450,8 @@
       <c r="P81" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q81" s="2" t="n">
-        <v>0</v>
+      <c r="Q81" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,8 +6464,8 @@
       <c r="P82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q82" s="2" t="n">
-        <v>0</v>
+      <c r="Q82" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,8 +6478,8 @@
       <c r="P83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q83" s="2" t="n">
-        <v>0</v>
+      <c r="Q83" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6485,8 +6492,8 @@
       <c r="P84" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q84" s="2" t="n">
-        <v>0</v>
+      <c r="Q84" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6499,8 +6506,8 @@
       <c r="P85" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q85" s="2" t="n">
-        <v>0</v>
+      <c r="Q85" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6513,8 +6520,8 @@
       <c r="P86" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q86" s="2" t="n">
-        <v>0</v>
+      <c r="Q86" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6527,8 +6534,8 @@
       <c r="P87" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q87" s="2" t="n">
-        <v>0</v>
+      <c r="Q87" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6541,8 +6548,8 @@
       <c r="P88" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q88" s="2" t="n">
-        <v>0</v>
+      <c r="Q88" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6555,8 +6562,8 @@
       <c r="P89" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q89" s="2" t="n">
-        <v>0</v>
+      <c r="Q89" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6569,8 +6576,8 @@
       <c r="P90" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q90" s="2" t="n">
-        <v>0</v>
+      <c r="Q90" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6583,8 +6590,8 @@
       <c r="P91" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q91" s="2" t="n">
-        <v>0</v>
+      <c r="Q91" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6597,8 +6604,8 @@
       <c r="P92" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q92" s="2" t="n">
-        <v>0</v>
+      <c r="Q92" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6611,8 +6618,8 @@
       <c r="P93" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q93" s="2" t="n">
-        <v>0</v>
+      <c r="Q93" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6625,8 +6632,8 @@
       <c r="P94" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q94" s="2" t="n">
-        <v>0</v>
+      <c r="Q94" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6639,8 +6646,8 @@
       <c r="P95" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q95" s="2" t="n">
-        <v>0</v>
+      <c r="Q95" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,8 +6663,8 @@
       <c r="P96" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q96" s="2" t="n">
-        <v>0</v>
+      <c r="Q96" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6673,8 +6680,8 @@
       <c r="P97" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q97" s="2" t="n">
-        <v>0</v>
+      <c r="Q97" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6687,8 +6694,8 @@
       <c r="P98" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q98" s="2" t="n">
-        <v>0</v>
+      <c r="Q98" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6701,8 +6708,8 @@
       <c r="P99" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q99" s="2" t="n">
-        <v>0</v>
+      <c r="Q99" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6715,8 +6722,8 @@
       <c r="P100" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q100" s="2" t="n">
-        <v>0</v>
+      <c r="Q100" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6729,8 +6736,8 @@
       <c r="P101" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q101" s="2" t="n">
-        <v>0</v>
+      <c r="Q101" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6743,8 +6750,8 @@
       <c r="P102" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q102" s="2" t="n">
-        <v>0</v>
+      <c r="Q102" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6757,8 +6764,8 @@
       <c r="P103" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q103" s="2" t="n">
-        <v>0</v>
+      <c r="Q103" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6771,8 +6778,8 @@
       <c r="P104" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q104" s="2" t="n">
-        <v>0</v>
+      <c r="Q104" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6785,8 +6792,8 @@
       <c r="P105" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q105" s="2" t="n">
-        <v>0</v>
+      <c r="Q105" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6799,8 +6806,8 @@
       <c r="P106" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q106" s="2" t="n">
-        <v>0</v>
+      <c r="Q106" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6813,8 +6820,8 @@
       <c r="P107" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q107" s="2" t="n">
-        <v>0</v>
+      <c r="Q107" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,8 +6834,8 @@
       <c r="P108" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q108" s="2" t="n">
-        <v>0</v>
+      <c r="Q108" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6841,8 +6848,8 @@
       <c r="P109" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q109" s="2" t="n">
-        <v>0</v>
+      <c r="Q109" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6855,8 +6862,8 @@
       <c r="P110" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q110" s="2" t="n">
-        <v>0</v>
+      <c r="Q110" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,8 +6876,8 @@
       <c r="P111" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q111" s="2" t="n">
-        <v>0</v>
+      <c r="Q111" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6883,8 +6890,8 @@
       <c r="P112" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q112" s="2" t="n">
-        <v>0</v>
+      <c r="Q112" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6897,8 +6904,8 @@
       <c r="P113" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q113" s="2" t="n">
-        <v>0</v>
+      <c r="Q113" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6911,8 +6918,8 @@
       <c r="P114" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q114" s="2" t="n">
-        <v>0</v>
+      <c r="Q114" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6925,8 +6932,8 @@
       <c r="P115" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q115" s="2" t="n">
-        <v>0</v>
+      <c r="Q115" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6939,8 +6946,8 @@
       <c r="P116" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q116" s="2" t="n">
-        <v>0</v>
+      <c r="Q116" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6953,8 +6960,8 @@
       <c r="P117" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q117" s="2" t="n">
-        <v>0</v>
+      <c r="Q117" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6967,8 +6974,8 @@
       <c r="P118" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q118" s="2" t="n">
-        <v>0</v>
+      <c r="Q118" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6981,8 +6988,8 @@
       <c r="P119" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q119" s="2" t="n">
-        <v>0</v>
+      <c r="Q119" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6995,8 +7002,8 @@
       <c r="P120" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q120" s="2" t="n">
-        <v>0</v>
+      <c r="Q120" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7009,8 +7016,8 @@
       <c r="P121" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q121" s="2" t="n">
-        <v>0</v>
+      <c r="Q121" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7023,8 +7030,8 @@
       <c r="P122" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q122" s="2" t="n">
-        <v>0</v>
+      <c r="Q122" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7037,8 +7044,8 @@
       <c r="P123" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q123" s="2" t="n">
-        <v>0</v>
+      <c r="Q123" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7051,8 +7058,8 @@
       <c r="P124" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q124" s="2" t="n">
-        <v>0</v>
+      <c r="Q124" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7065,8 +7072,8 @@
       <c r="P125" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q125" s="2" t="n">
-        <v>0</v>
+      <c r="Q125" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7079,8 +7086,8 @@
       <c r="P126" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q126" s="2" t="n">
-        <v>0</v>
+      <c r="Q126" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7093,8 +7100,8 @@
       <c r="P127" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q127" s="2" t="n">
-        <v>0</v>
+      <c r="Q127" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7107,8 +7114,8 @@
       <c r="P128" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q128" s="2" t="n">
-        <v>0</v>
+      <c r="Q128" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7124,11 +7131,17 @@
       <c r="P129" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q129" s="2" t="n">
-        <v>0</v>
+      <c r="Q129" s="6" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E65 I2:I33 M2:M33 Q2:Q129" type="list">
+      <formula1>"+60,+55,+50,+45,+40,+35,+30,+25,+20,+15,+10,+5,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7146,14 +7159,14 @@
   </sheetPr>
   <dimension ref="A1:Z129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K51" activeCellId="0" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="1" width="4.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="2" width="4.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="37.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7245,6 +7258,9 @@
         <f aca="false">Channels!B2</f>
         <v>KickIn</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -7255,6 +7271,9 @@
         <f aca="false">Channels!B3</f>
         <v>KickOut</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -7265,6 +7284,9 @@
         <f aca="false">Channels!B4</f>
         <v>SnTop</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -7275,6 +7297,9 @@
         <f aca="false">Channels!B5</f>
         <v>SnBot</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -7285,6 +7310,9 @@
         <f aca="false">Channels!B6</f>
         <v>Hat</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -7295,6 +7323,9 @@
         <f aca="false">Channels!B7</f>
         <v>Rack1</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -7305,6 +7336,9 @@
         <f aca="false">Channels!B8</f>
         <v>Rack2</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -7315,6 +7349,9 @@
         <f aca="false">Channels!B9</f>
         <v>Floor1</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -7325,6 +7362,9 @@
         <f aca="false">Channels!B10</f>
         <v>Floor2</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -7335,6 +7375,9 @@
         <f aca="false">Channels!B11</f>
         <v>Ride</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -7345,6 +7388,9 @@
         <f aca="false">Channels!B12</f>
         <v>OH L</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -7354,6 +7400,9 @@
       <c r="B13" s="1" t="str">
         <f aca="false">Channels!B13</f>
         <v>OH R</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7375,6 +7424,9 @@
         <f aca="false">Channels!B15</f>
         <v>Cajon</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -7405,6 +7457,9 @@
         <f aca="false">Channels!B18</f>
         <v>BassDI</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -7415,6 +7470,9 @@
         <f aca="false">Channels!B19</f>
         <v>BassMi</v>
       </c>
+      <c r="E19" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -7425,6 +7483,9 @@
         <f aca="false">Channels!B20</f>
         <v>EGit1L</v>
       </c>
+      <c r="F20" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -7435,6 +7496,9 @@
         <f aca="false">Channels!B21</f>
         <v>EGit1R</v>
       </c>
+      <c r="F21" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -7445,6 +7509,9 @@
         <f aca="false">Channels!B22</f>
         <v>EGit2L</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -7455,6 +7522,9 @@
         <f aca="false">Channels!B23</f>
         <v>EGit2R</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -7465,6 +7535,9 @@
         <f aca="false">Channels!B24</f>
         <v>EGit3L</v>
       </c>
+      <c r="F24" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -7475,6 +7548,9 @@
         <f aca="false">Channels!B25</f>
         <v>EGit3R</v>
       </c>
+      <c r="F25" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -7484,6 +7560,9 @@
       <c r="B26" s="1" t="str">
         <f aca="false">Channels!B26</f>
         <v>Accu1L</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7495,6 +7574,9 @@
         <f aca="false">Channels!B27</f>
         <v>Accu1R</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -7505,6 +7587,9 @@
         <f aca="false">Channels!B28</f>
         <v>Accu2</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -7515,6 +7600,9 @@
         <f aca="false">Channels!B29</f>
         <v>Accu3</v>
       </c>
+      <c r="G29" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
@@ -7525,6 +7613,9 @@
         <f aca="false">Channels!B30</f>
         <v>Key1L</v>
       </c>
+      <c r="H30" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
@@ -7535,6 +7626,9 @@
         <f aca="false">Channels!B31</f>
         <v>Key1R</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
@@ -7545,6 +7639,9 @@
         <f aca="false">Channels!B32</f>
         <v>Key2L</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
@@ -7555,6 +7652,9 @@
         <f aca="false">Channels!B33</f>
         <v>Key2R</v>
       </c>
+      <c r="H33" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
@@ -7565,6 +7665,9 @@
         <f aca="false">Channels!B34</f>
         <v>Key3L</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -7575,6 +7678,9 @@
         <f aca="false">Channels!B35</f>
         <v>Key3R</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -7585,6 +7691,9 @@
         <f aca="false">Channels!B36</f>
         <v>Key4L</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -7595,6 +7704,9 @@
         <f aca="false">Channels!B37</f>
         <v>Key4R</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -7605,6 +7717,9 @@
         <f aca="false">Channels!B38</f>
         <v>Divrs1</v>
       </c>
+      <c r="I38" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
@@ -7615,6 +7730,9 @@
         <f aca="false">Channels!B39</f>
         <v>Divrs2</v>
       </c>
+      <c r="I39" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
@@ -7625,6 +7743,9 @@
         <f aca="false">Channels!B40</f>
         <v>Divrs3</v>
       </c>
+      <c r="I40" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
@@ -7635,6 +7756,9 @@
         <f aca="false">Channels!B41</f>
         <v>Divrs4</v>
       </c>
+      <c r="I41" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
@@ -7645,6 +7769,9 @@
         <f aca="false">Channels!B42</f>
         <v>Lead1</v>
       </c>
+      <c r="J42" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
@@ -7655,6 +7782,9 @@
         <f aca="false">Channels!B43</f>
         <v>Lead2</v>
       </c>
+      <c r="J43" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
@@ -7665,6 +7795,9 @@
         <f aca="false">Channels!B44</f>
         <v>Lead3</v>
       </c>
+      <c r="J44" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -7675,6 +7808,9 @@
         <f aca="false">Channels!B45</f>
         <v>Lead4</v>
       </c>
+      <c r="J45" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
@@ -7685,6 +7821,9 @@
         <f aca="false">Channels!B46</f>
         <v>BV1</v>
       </c>
+      <c r="K46" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -7695,6 +7834,9 @@
         <f aca="false">Channels!B47</f>
         <v>BV2</v>
       </c>
+      <c r="K47" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
@@ -7705,6 +7847,9 @@
         <f aca="false">Channels!B48</f>
         <v>BV3</v>
       </c>
+      <c r="K48" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
@@ -7714,6 +7859,9 @@
       <c r="B49" s="1" t="str">
         <f aca="false">Channels!B49</f>
         <v>BV4</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8547,24 +8695,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
mute group handling added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="128">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -516,7 +516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -550,6 +550,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO16" activeCellId="0" sqref="AO16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL5" activeCellId="0" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -887,6 +891,16 @@
       <c r="L2" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -919,6 +933,16 @@
       <c r="L3" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -951,6 +975,16 @@
       <c r="L4" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="9"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -983,6 +1017,16 @@
       <c r="L5" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -1015,6 +1059,16 @@
       <c r="L6" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -1047,6 +1101,16 @@
       <c r="L7" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -1079,6 +1143,16 @@
       <c r="L8" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -1109,6 +1183,16 @@
         <v>43</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4792,49 +4876,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>105</v>
       </c>
       <c r="F1" s="5"/>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>108</v>
       </c>
       <c r="J1" s="5"/>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="14" t="s">
         <v>111</v>
       </c>
       <c r="N1" s="5"/>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="15" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comment fixed in Cell A1 fixed
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -321,7 +321,7 @@
     <t xml:space="preserve">BV4</t>
   </si>
   <si>
-    <t xml:space="preserve">Indication Start/End Channel
+    <t xml:space="preserve">Indication Start/End Socket
 For
 Mixrack / Expanders
 </t>
@@ -700,7 +700,7 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -4960,8 +4960,8 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
first time open default tab selected
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -700,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4960,7 +4960,7 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
group naming and coloring added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="48V &amp; Pad" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Misc" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sockets" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Groups" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Misc" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="434">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -388,6 +389,930 @@
   </si>
   <si>
     <t xml:space="preserve">Slink-DX2 End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCA Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCA Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mono Auxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aux Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aux Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stereo Auxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StAux Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StAux Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mono Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stereo Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StGroup Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StGroup Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mono Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrix Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrix Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stereo Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StMatrix Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StMatrix Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egitrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccGtr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAUX31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSGRP31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSMTX31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMAUX62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMGRP62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMMTX62</t>
   </si>
   <si>
     <t xml:space="preserve">Property</t>
@@ -444,7 +1369,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,7 +1385,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB7B3CA"/>
-        <bgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
     <fill>
@@ -472,16 +1397,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAFD095"/>
-        <bgColor rgb="FF92D050"/>
+        <bgColor rgb="FFB3B3B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3B3B3"/>
+        <bgColor rgb="FFB7B3CA"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -510,7 +1448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,6 +1503,34 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -666,9 +1632,9 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFB66C"/>
@@ -700,8 +1666,8 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4960,7 +5926,7 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8013,6 +8979,2981 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AA65"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="12.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="T1" s="15"/>
+      <c r="U1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA3" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y4" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA4" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y5" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="W6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y6" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA6" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA7" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="S8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="W8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y8" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA8" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="R9" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="S9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="V9" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="W9" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y9" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA9" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="R10" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="S10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="V10" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="W10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y10" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA10" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="R11" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="V11" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="W11" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y11" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA11" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="S12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="V12" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="W12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="16" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z12" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA12" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="R13" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="S13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="W13" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z13" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA13" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="O14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="S14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="V14" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="W14" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y14" s="16" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA14" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="R15" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="V15" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="W15" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z15" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA15" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="R16" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="S16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="V16" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="W16" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y16" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z16" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA16" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="O17" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="S17" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="V17" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="W17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y17" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z17" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA17" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="R18" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="S18" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="V18" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="W18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y18" s="16" t="n">
+        <v>17</v>
+      </c>
+      <c r="Z18" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA18" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="R19" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="V19" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="W19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y19" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z19" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA19" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="R20" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="S20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="V20" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="W20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y20" s="16" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z20" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA20" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="R21" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="S21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="V21" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="W21" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y21" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z21" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA21" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="R22" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="S22" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="V22" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="W22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y22" s="16" t="n">
+        <v>21</v>
+      </c>
+      <c r="Z22" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA22" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="V23" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="W23" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y23" s="16" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z23" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA23" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="O24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="S24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="V24" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="W24" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y24" s="16" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z24" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="AA24" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="V25" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="W25" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z25" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA25" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="O26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="S26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="V26" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="W26" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y26" s="16" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z26" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="AA26" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="S27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="V27" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="W27" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y27" s="16" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z27" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA27" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="O28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="V28" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="W28" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y28" s="16" t="n">
+        <v>27</v>
+      </c>
+      <c r="Z28" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="AA28" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="K29" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="O29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="S29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="V29" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="W29" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y29" s="16" t="n">
+        <v>28</v>
+      </c>
+      <c r="Z29" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="AA29" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="K30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="O30" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="R30" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="S30" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="V30" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="W30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y30" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="Z30" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA30" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="O31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="S31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="V31" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="W31" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y31" s="16" t="n">
+        <v>30</v>
+      </c>
+      <c r="Z31" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA31" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="O32" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="R32" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="S32" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="V32" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="W32" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y32" s="16" t="n">
+        <v>31</v>
+      </c>
+      <c r="Z32" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA32" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" s="19"/>
+      <c r="M33" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="O33" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="S33" s="19"/>
+      <c r="U33" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="V33" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="W33" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M34" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="O34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U34" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="V34" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="W34" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="16" t="n">
+        <v>34</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" s="16" t="n">
+        <v>34</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="O35" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U35" s="16" t="n">
+        <v>34</v>
+      </c>
+      <c r="V35" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="W35" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M36" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="O36" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U36" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="V36" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="W36" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M37" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="O37" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U37" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="V37" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="W37" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="16" t="n">
+        <v>37</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M38" s="16" t="n">
+        <v>37</v>
+      </c>
+      <c r="N38" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="O38" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U38" s="16" t="n">
+        <v>37</v>
+      </c>
+      <c r="V38" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="W38" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="16" t="n">
+        <v>38</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M39" s="16" t="n">
+        <v>38</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="O39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U39" s="16" t="n">
+        <v>38</v>
+      </c>
+      <c r="V39" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="W39" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M40" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="N40" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="O40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U40" s="16" t="n">
+        <v>39</v>
+      </c>
+      <c r="V40" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="W40" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="16" t="n">
+        <v>40</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M41" s="16" t="n">
+        <v>40</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="O41" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U41" s="16" t="n">
+        <v>40</v>
+      </c>
+      <c r="V41" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="W41" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="16" t="n">
+        <v>41</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M42" s="16" t="n">
+        <v>41</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="O42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U42" s="16" t="n">
+        <v>41</v>
+      </c>
+      <c r="V42" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="W42" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="16" t="n">
+        <v>42</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M43" s="16" t="n">
+        <v>42</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U43" s="16" t="n">
+        <v>42</v>
+      </c>
+      <c r="V43" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="W43" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="16" t="n">
+        <v>43</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M44" s="16" t="n">
+        <v>43</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="O44" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U44" s="16" t="n">
+        <v>43</v>
+      </c>
+      <c r="V44" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="W44" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="16" t="n">
+        <v>44</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M45" s="16" t="n">
+        <v>44</v>
+      </c>
+      <c r="N45" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="O45" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U45" s="16" t="n">
+        <v>44</v>
+      </c>
+      <c r="V45" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="W45" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="16" t="n">
+        <v>45</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M46" s="16" t="n">
+        <v>45</v>
+      </c>
+      <c r="N46" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="O46" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U46" s="16" t="n">
+        <v>45</v>
+      </c>
+      <c r="V46" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="W46" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="16" t="n">
+        <v>46</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M47" s="16" t="n">
+        <v>46</v>
+      </c>
+      <c r="N47" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="O47" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U47" s="16" t="n">
+        <v>46</v>
+      </c>
+      <c r="V47" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="W47" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="16" t="n">
+        <v>47</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M48" s="16" t="n">
+        <v>47</v>
+      </c>
+      <c r="N48" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="O48" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U48" s="16" t="n">
+        <v>47</v>
+      </c>
+      <c r="V48" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="W48" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="16" t="n">
+        <v>48</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M49" s="16" t="n">
+        <v>48</v>
+      </c>
+      <c r="N49" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="O49" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U49" s="16" t="n">
+        <v>48</v>
+      </c>
+      <c r="V49" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="W49" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="16" t="n">
+        <v>49</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M50" s="16" t="n">
+        <v>49</v>
+      </c>
+      <c r="N50" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="O50" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U50" s="16" t="n">
+        <v>49</v>
+      </c>
+      <c r="V50" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="W50" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M51" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="N51" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="O51" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U51" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="V51" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="W51" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="16" t="n">
+        <v>51</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M52" s="16" t="n">
+        <v>51</v>
+      </c>
+      <c r="N52" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="O52" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U52" s="16" t="n">
+        <v>51</v>
+      </c>
+      <c r="V52" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="W52" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="16" t="n">
+        <v>52</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M53" s="16" t="n">
+        <v>52</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="O53" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U53" s="16" t="n">
+        <v>52</v>
+      </c>
+      <c r="V53" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="W53" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="16" t="n">
+        <v>53</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M54" s="16" t="n">
+        <v>53</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="O54" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U54" s="16" t="n">
+        <v>53</v>
+      </c>
+      <c r="V54" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="W54" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="16" t="n">
+        <v>54</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M55" s="16" t="n">
+        <v>54</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="O55" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U55" s="16" t="n">
+        <v>54</v>
+      </c>
+      <c r="V55" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="W55" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M56" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="O56" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U56" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="V56" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="W56" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="16" t="n">
+        <v>56</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M57" s="16" t="n">
+        <v>56</v>
+      </c>
+      <c r="N57" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="O57" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U57" s="16" t="n">
+        <v>56</v>
+      </c>
+      <c r="V57" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="W57" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="16" t="n">
+        <v>57</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M58" s="16" t="n">
+        <v>57</v>
+      </c>
+      <c r="N58" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="O58" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U58" s="16" t="n">
+        <v>57</v>
+      </c>
+      <c r="V58" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="W58" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="16" t="n">
+        <v>58</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M59" s="16" t="n">
+        <v>58</v>
+      </c>
+      <c r="N59" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="O59" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U59" s="16" t="n">
+        <v>58</v>
+      </c>
+      <c r="V59" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="W59" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="16" t="n">
+        <v>59</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M60" s="16" t="n">
+        <v>59</v>
+      </c>
+      <c r="N60" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="O60" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U60" s="16" t="n">
+        <v>59</v>
+      </c>
+      <c r="V60" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="W60" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="16" t="n">
+        <v>60</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M61" s="16" t="n">
+        <v>60</v>
+      </c>
+      <c r="N61" s="17" t="s">
+        <v>421</v>
+      </c>
+      <c r="O61" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U61" s="16" t="n">
+        <v>60</v>
+      </c>
+      <c r="V61" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="W61" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="16" t="n">
+        <v>61</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M62" s="16" t="n">
+        <v>61</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="O62" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U62" s="16" t="n">
+        <v>61</v>
+      </c>
+      <c r="V62" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="W62" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="16" t="n">
+        <v>62</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M63" s="16" t="n">
+        <v>62</v>
+      </c>
+      <c r="N63" s="17" t="s">
+        <v>427</v>
+      </c>
+      <c r="O63" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U63" s="16" t="n">
+        <v>62</v>
+      </c>
+      <c r="V63" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="W63" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F64" s="20"/>
+      <c r="G64" s="19"/>
+      <c r="O64" s="19"/>
+      <c r="W64" s="19"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G65" s="19"/>
+      <c r="O65" s="19"/>
+      <c r="W65" s="19"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C25 G2:G65 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"purple"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"light blue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"green"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"red"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>"black"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>"yellow"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>"blue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C25 G2:G34 K2:K33 O2:O65 S2:S33 W2:W65 AA2:AA33 G35:G65" type="list">
+      <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -8028,24 +11969,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>429</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>430</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>432</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
hint for mixer config sheet added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="514">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -1551,6 +1551,11 @@
   </si>
   <si>
     <t xml:space="preserve">Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a report from the „Groups“ sheet. It does not change the Mixer Config. 
+When you change the default name in the „Groups“ sheet, 
+the corresponding value is increased here.</t>
   </si>
   <si>
     <t xml:space="preserve">Property</t>
@@ -1577,7 +1582,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1629,8 +1634,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1670,7 +1682,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3838"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1695,6 +1707,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1739,7 +1757,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1889,6 +1907,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2117,7 +2143,7 @@
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF7030A0"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -2134,9 +2160,9 @@
   <dimension ref="A1:XFD131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
@@ -27847,10 +27873,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27915,6 +27941,16 @@
         <f aca="false">Groups!AG65</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="38" t="s">
+        <v>508</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -27947,24 +27983,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="C1" s="38" t="s">
         <v>510</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hint for mixer config sheet updated
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -1910,7 +1910,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -27872,7 +27872,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27938,7 +27938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="99.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
         <v>508</v>
       </c>

</xml_diff>

<commit_message>
excel formula fixed at AT2
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="514">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -2156,11 +2156,11 @@
   <dimension ref="A1:XFD131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="BT10" activeCellId="0" sqref="BT10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2455,8 +2455,9 @@
       <c r="AP2" s="10"/>
       <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
-      <c r="AT2" s="2" t="s">
-        <v>46</v>
+      <c r="AT2" s="2" t="str">
+        <f aca="false">IF(L2="x","x","")</f>
+        <v>x</v>
       </c>
       <c r="AU2" s="2" t="str">
         <f aca="false">IF(M2="x","x","")</f>

</xml_diff>

<commit_message>
doc updated empty cell handling added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -19831,12 +19831,12 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27977,7 +27977,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dont care feature for channels sheet added
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -2158,12 +2158,12 @@
   </sheetPr>
   <dimension ref="A1:XFD131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BT10" activeCellId="0" sqref="BT10"/>
+      <selection pane="bottomRight" activeCell="J2" activeCellId="0" sqref="J2:J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2427,13 +2427,13 @@
       <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E2" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="2" t="n">
@@ -2442,7 +2442,7 @@
       <c r="I2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -2573,13 +2573,13 @@
       <c r="C3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="2" t="n">
@@ -2588,7 +2588,7 @@
       <c r="I3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -2719,13 +2719,13 @@
       <c r="C4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="2" t="n">
@@ -2734,7 +2734,7 @@
       <c r="I4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -2865,13 +2865,13 @@
       <c r="C5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="2" t="n">
@@ -2880,7 +2880,7 @@
       <c r="I5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -3011,13 +3011,13 @@
       <c r="C6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -3026,7 +3026,7 @@
       <c r="I6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -3157,13 +3157,13 @@
       <c r="C7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -3172,7 +3172,7 @@
       <c r="I7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -3303,13 +3303,13 @@
       <c r="C8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="2" t="n">
@@ -3318,7 +3318,7 @@
       <c r="I8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -3449,13 +3449,13 @@
       <c r="C9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="2" t="n">
@@ -3464,7 +3464,7 @@
       <c r="I9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -3595,13 +3595,13 @@
       <c r="C10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="2" t="n">
@@ -3610,7 +3610,7 @@
       <c r="I10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -3734,13 +3734,13 @@
       <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="2" t="n">
@@ -3749,7 +3749,7 @@
       <c r="I11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -3873,13 +3873,13 @@
       <c r="C12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="2" t="n">
@@ -3888,7 +3888,7 @@
       <c r="I12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -4012,13 +4012,13 @@
       <c r="C13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G13" s="2" t="n">
@@ -4027,7 +4027,7 @@
       <c r="I13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -4151,13 +4151,13 @@
       <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G14" s="2" t="n">
@@ -4166,7 +4166,7 @@
       <c r="I14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="10" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -4290,13 +4290,13 @@
       <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="2" t="n">
@@ -4305,7 +4305,7 @@
       <c r="I15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK15" s="2" t="s">
@@ -4426,13 +4426,13 @@
       <c r="C16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G16" s="2" t="n">
@@ -4441,7 +4441,7 @@
       <c r="I16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK16" s="2" t="s">
@@ -4562,13 +4562,13 @@
       <c r="C17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="2" t="n">
@@ -4577,7 +4577,7 @@
       <c r="I17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK17" s="2" t="s">
@@ -4698,13 +4698,13 @@
       <c r="C18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G18" s="2" t="n">
@@ -4713,7 +4713,7 @@
       <c r="I18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="10" t="s">
         <v>44</v>
       </c>
       <c r="N18" s="2" t="s">
@@ -4837,13 +4837,13 @@
       <c r="C19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="2" t="n">
@@ -4852,7 +4852,7 @@
       <c r="I19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="10" t="s">
         <v>44</v>
       </c>
       <c r="N19" s="2" t="s">
@@ -4976,13 +4976,13 @@
       <c r="C20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G20" s="2" t="n">
@@ -4991,7 +4991,7 @@
       <c r="I20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O20" s="2" t="s">
@@ -5115,13 +5115,13 @@
       <c r="C21" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="2" t="n">
@@ -5130,7 +5130,7 @@
       <c r="I21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -5254,13 +5254,13 @@
       <c r="C22" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="2" t="n">
@@ -5269,7 +5269,7 @@
       <c r="I22" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O22" s="2" t="s">
@@ -5393,13 +5393,13 @@
       <c r="C23" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="2" t="n">
@@ -5408,7 +5408,7 @@
       <c r="I23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -5532,13 +5532,13 @@
       <c r="C24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G24" s="2" t="n">
@@ -5547,7 +5547,7 @@
       <c r="I24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O24" s="2" t="s">
@@ -5671,13 +5671,13 @@
       <c r="C25" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="2" t="n">
@@ -5686,7 +5686,7 @@
       <c r="I25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="10" t="s">
         <v>44</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -5810,13 +5810,13 @@
       <c r="C26" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G26" s="2" t="n">
@@ -5825,7 +5825,7 @@
       <c r="I26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P26" s="2" t="s">
@@ -5949,13 +5949,13 @@
       <c r="C27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G27" s="2" t="n">
@@ -5964,7 +5964,7 @@
       <c r="I27" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P27" s="2" t="s">
@@ -6088,13 +6088,13 @@
       <c r="C28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G28" s="2" t="n">
@@ -6103,7 +6103,7 @@
       <c r="I28" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P28" s="2" t="s">
@@ -6227,13 +6227,13 @@
       <c r="C29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E29" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G29" s="2" t="n">
@@ -6242,7 +6242,7 @@
       <c r="I29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P29" s="2" t="s">
@@ -6366,13 +6366,13 @@
       <c r="C30" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G30" s="2" t="n">
@@ -6381,7 +6381,7 @@
       <c r="I30" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q30" s="2" t="s">
@@ -6505,13 +6505,13 @@
       <c r="C31" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G31" s="2" t="n">
@@ -6520,7 +6520,7 @@
       <c r="I31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q31" s="2" t="s">
@@ -6644,13 +6644,13 @@
       <c r="C32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G32" s="2" t="n">
@@ -6659,7 +6659,7 @@
       <c r="I32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q32" s="2" t="s">
@@ -6783,13 +6783,13 @@
       <c r="C33" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G33" s="2" t="n">
@@ -6798,7 +6798,7 @@
       <c r="I33" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q33" s="2" t="s">
@@ -6922,13 +6922,13 @@
       <c r="C34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E34" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G34" s="2" t="n">
@@ -6937,7 +6937,7 @@
       <c r="I34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q34" s="2" t="s">
@@ -7061,13 +7061,13 @@
       <c r="C35" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G35" s="2" t="n">
@@ -7076,7 +7076,7 @@
       <c r="I35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q35" s="2" t="s">
@@ -7200,13 +7200,13 @@
       <c r="C36" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E36" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G36" s="2" t="n">
@@ -7215,7 +7215,7 @@
       <c r="I36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q36" s="2" t="s">
@@ -7339,13 +7339,13 @@
       <c r="C37" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E37" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G37" s="2" t="n">
@@ -7354,7 +7354,7 @@
       <c r="I37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="10" t="s">
         <v>44</v>
       </c>
       <c r="Q37" s="2" t="s">
@@ -7478,13 +7478,13 @@
       <c r="C38" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G38" s="2" t="n">
@@ -7493,7 +7493,7 @@
       <c r="I38" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK38" s="2" t="s">
@@ -7614,13 +7614,13 @@
       <c r="C39" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G39" s="2" t="n">
@@ -7629,7 +7629,7 @@
       <c r="I39" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK39" s="2" t="s">
@@ -7750,13 +7750,13 @@
       <c r="C40" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G40" s="2" t="n">
@@ -7765,7 +7765,7 @@
       <c r="I40" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK40" s="2" t="s">
@@ -7886,13 +7886,13 @@
       <c r="C41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E41" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G41" s="2" t="n">
@@ -7901,7 +7901,7 @@
       <c r="I41" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AK41" s="2" t="s">
@@ -8022,13 +8022,13 @@
       <c r="C42" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E42" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G42" s="2" t="n">
@@ -8037,7 +8037,7 @@
       <c r="I42" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" s="10" t="s">
         <v>44</v>
       </c>
       <c r="R42" s="2" t="s">
@@ -8161,13 +8161,13 @@
       <c r="C43" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E43" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G43" s="2" t="n">
@@ -8176,7 +8176,7 @@
       <c r="I43" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="10" t="s">
         <v>44</v>
       </c>
       <c r="R43" s="2" t="s">
@@ -8300,13 +8300,13 @@
       <c r="C44" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E44" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G44" s="2" t="n">
@@ -8315,7 +8315,7 @@
       <c r="I44" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="10" t="s">
         <v>44</v>
       </c>
       <c r="R44" s="2" t="s">
@@ -8439,13 +8439,13 @@
       <c r="C45" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E45" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G45" s="2" t="n">
@@ -8454,7 +8454,7 @@
       <c r="I45" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="10" t="s">
         <v>44</v>
       </c>
       <c r="R45" s="2" t="s">
@@ -8578,13 +8578,13 @@
       <c r="C46" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E46" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G46" s="2" t="n">
@@ -8593,7 +8593,7 @@
       <c r="I46" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="J46" s="10" t="s">
         <v>44</v>
       </c>
       <c r="S46" s="2" t="s">
@@ -8717,13 +8717,13 @@
       <c r="C47" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E47" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G47" s="2" t="n">
@@ -8732,7 +8732,7 @@
       <c r="I47" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="10" t="s">
         <v>44</v>
       </c>
       <c r="S47" s="2" t="s">
@@ -8856,13 +8856,13 @@
       <c r="C48" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E48" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G48" s="2" t="n">
@@ -8871,7 +8871,7 @@
       <c r="I48" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="10" t="s">
         <v>44</v>
       </c>
       <c r="S48" s="2" t="s">
@@ -8995,13 +8995,13 @@
       <c r="C49" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E49" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G49" s="2" t="n">
@@ -9010,7 +9010,7 @@
       <c r="I49" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="J49" s="10" t="s">
         <v>44</v>
       </c>
       <c r="S49" s="2" t="s">
@@ -9134,13 +9134,13 @@
       <c r="C50" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E50" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G50" s="2" t="n">
@@ -9149,7 +9149,7 @@
       <c r="I50" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="J50" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT50" s="2" t="str">
@@ -9267,13 +9267,13 @@
       <c r="C51" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E51" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G51" s="2" t="n">
@@ -9282,7 +9282,7 @@
       <c r="I51" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="J51" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT51" s="2" t="str">
@@ -9400,13 +9400,13 @@
       <c r="C52" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E52" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G52" s="2" t="n">
@@ -9415,7 +9415,7 @@
       <c r="I52" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="J52" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT52" s="2" t="str">
@@ -9533,13 +9533,13 @@
       <c r="C53" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E53" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G53" s="2" t="n">
@@ -9548,7 +9548,7 @@
       <c r="I53" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="J53" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT53" s="2" t="str">
@@ -9666,13 +9666,13 @@
       <c r="C54" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E54" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G54" s="2" t="n">
@@ -9681,7 +9681,7 @@
       <c r="I54" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT54" s="2" t="str">
@@ -9799,13 +9799,13 @@
       <c r="C55" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E55" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G55" s="2" t="n">
@@ -9814,7 +9814,7 @@
       <c r="I55" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="J55" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT55" s="2" t="str">
@@ -9932,13 +9932,13 @@
       <c r="C56" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E56" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G56" s="2" t="n">
@@ -9947,7 +9947,7 @@
       <c r="I56" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="J56" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT56" s="2" t="str">
@@ -10065,13 +10065,13 @@
       <c r="C57" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E57" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G57" s="2" t="n">
@@ -10080,7 +10080,7 @@
       <c r="I57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="J57" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT57" s="2" t="str">
@@ -10198,13 +10198,13 @@
       <c r="C58" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E58" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G58" s="2" t="n">
@@ -10213,7 +10213,7 @@
       <c r="I58" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="J58" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT58" s="2" t="str">
@@ -10331,13 +10331,13 @@
       <c r="C59" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E59" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G59" s="2" t="n">
@@ -10346,7 +10346,7 @@
       <c r="I59" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="J59" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT59" s="2" t="str">
@@ -10464,13 +10464,13 @@
       <c r="C60" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E60" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G60" s="2" t="n">
@@ -10479,7 +10479,7 @@
       <c r="I60" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="J60" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT60" s="2" t="str">
@@ -10597,13 +10597,13 @@
       <c r="C61" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E61" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G61" s="2" t="n">
@@ -10612,7 +10612,7 @@
       <c r="I61" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="J61" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT61" s="2" t="str">
@@ -10730,13 +10730,13 @@
       <c r="C62" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E62" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G62" s="2" t="n">
@@ -10745,7 +10745,7 @@
       <c r="I62" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J62" s="2" t="s">
+      <c r="J62" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT62" s="2" t="str">
@@ -10863,13 +10863,13 @@
       <c r="C63" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E63" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G63" s="2" t="n">
@@ -10878,7 +10878,7 @@
       <c r="I63" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="J63" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT63" s="2" t="str">
@@ -10996,13 +10996,13 @@
       <c r="C64" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E64" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G64" s="2" t="n">
@@ -11011,7 +11011,7 @@
       <c r="I64" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J64" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT64" s="2" t="str">
@@ -11129,13 +11129,13 @@
       <c r="C65" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E65" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G65" s="2" t="n">
@@ -11144,7 +11144,7 @@
       <c r="I65" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="J65" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT65" s="2" t="str">
@@ -11262,13 +11262,13 @@
       <c r="C66" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E66" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G66" s="2" t="n">
@@ -11277,7 +11277,7 @@
       <c r="I66" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="J66" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT66" s="2" t="str">
@@ -11395,13 +11395,13 @@
       <c r="C67" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E67" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G67" s="2" t="n">
@@ -11410,7 +11410,7 @@
       <c r="I67" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="J67" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT67" s="2" t="str">
@@ -11528,13 +11528,13 @@
       <c r="C68" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E68" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G68" s="2" t="n">
@@ -11543,7 +11543,7 @@
       <c r="I68" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT68" s="2" t="str">
@@ -11661,13 +11661,13 @@
       <c r="C69" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E69" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G69" s="2" t="n">
@@ -11676,7 +11676,7 @@
       <c r="I69" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="J69" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT69" s="2" t="str">
@@ -11794,13 +11794,13 @@
       <c r="C70" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E70" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G70" s="2" t="n">
@@ -11809,7 +11809,7 @@
       <c r="I70" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="J70" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT70" s="2" t="str">
@@ -11927,13 +11927,13 @@
       <c r="C71" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E71" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G71" s="2" t="n">
@@ -11942,7 +11942,7 @@
       <c r="I71" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J71" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT71" s="2" t="str">
@@ -12060,13 +12060,13 @@
       <c r="C72" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E72" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G72" s="2" t="n">
@@ -12075,7 +12075,7 @@
       <c r="I72" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J72" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT72" s="2" t="str">
@@ -12193,13 +12193,13 @@
       <c r="C73" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E73" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G73" s="2" t="n">
@@ -12208,7 +12208,7 @@
       <c r="I73" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="J73" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT73" s="2" t="str">
@@ -12326,13 +12326,13 @@
       <c r="C74" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E74" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G74" s="2" t="n">
@@ -12341,7 +12341,7 @@
       <c r="I74" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="J74" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT74" s="2" t="str">
@@ -12459,13 +12459,13 @@
       <c r="C75" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E75" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G75" s="2" t="n">
@@ -12474,7 +12474,7 @@
       <c r="I75" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J75" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT75" s="2" t="str">
@@ -12592,13 +12592,13 @@
       <c r="C76" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E76" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G76" s="2" t="n">
@@ -12607,7 +12607,7 @@
       <c r="I76" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="J76" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT76" s="2" t="str">
@@ -12725,13 +12725,13 @@
       <c r="C77" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E77" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G77" s="2" t="n">
@@ -12740,7 +12740,7 @@
       <c r="I77" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="J77" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT77" s="2" t="str">
@@ -12858,13 +12858,13 @@
       <c r="C78" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E78" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G78" s="2" t="n">
@@ -12873,7 +12873,7 @@
       <c r="I78" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J78" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT78" s="2" t="str">
@@ -12991,13 +12991,13 @@
       <c r="C79" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E79" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G79" s="2" t="n">
@@ -13006,7 +13006,7 @@
       <c r="I79" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="J79" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT79" s="2" t="str">
@@ -13124,13 +13124,13 @@
       <c r="C80" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E80" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G80" s="2" t="n">
@@ -13139,7 +13139,7 @@
       <c r="I80" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J80" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT80" s="2" t="str">
@@ -13257,13 +13257,13 @@
       <c r="C81" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E81" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G81" s="2" t="n">
@@ -13272,7 +13272,7 @@
       <c r="I81" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="J81" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT81" s="2" t="str">
@@ -13390,13 +13390,13 @@
       <c r="C82" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E82" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G82" s="2" t="n">
@@ -13405,7 +13405,7 @@
       <c r="I82" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="J82" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT82" s="2" t="str">
@@ -13523,13 +13523,13 @@
       <c r="C83" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D83" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E83" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G83" s="2" t="n">
@@ -13538,7 +13538,7 @@
       <c r="I83" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="J83" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT83" s="2" t="str">
@@ -13656,13 +13656,13 @@
       <c r="C84" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E84" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G84" s="2" t="n">
@@ -13671,7 +13671,7 @@
       <c r="I84" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="J84" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT84" s="2" t="str">
@@ -13789,13 +13789,13 @@
       <c r="C85" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E85" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G85" s="2" t="n">
@@ -13804,7 +13804,7 @@
       <c r="I85" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="J85" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT85" s="2" t="str">
@@ -13922,13 +13922,13 @@
       <c r="C86" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E86" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G86" s="2" t="n">
@@ -13937,7 +13937,7 @@
       <c r="I86" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="J86" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT86" s="2" t="str">
@@ -14055,13 +14055,13 @@
       <c r="C87" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E87" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G87" s="2" t="n">
@@ -14070,7 +14070,7 @@
       <c r="I87" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="J87" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT87" s="2" t="str">
@@ -14188,13 +14188,13 @@
       <c r="C88" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E88" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G88" s="2" t="n">
@@ -14203,7 +14203,7 @@
       <c r="I88" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="J88" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT88" s="2" t="str">
@@ -14321,13 +14321,13 @@
       <c r="C89" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E89" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G89" s="2" t="n">
@@ -14336,7 +14336,7 @@
       <c r="I89" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J89" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT89" s="2" t="str">
@@ -14454,13 +14454,13 @@
       <c r="C90" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D90" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E90" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F90" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G90" s="2" t="n">
@@ -14469,7 +14469,7 @@
       <c r="I90" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J90" s="2" t="s">
+      <c r="J90" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT90" s="2" t="str">
@@ -14587,13 +14587,13 @@
       <c r="C91" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D91" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E91" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F91" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G91" s="2" t="n">
@@ -14602,7 +14602,7 @@
       <c r="I91" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J91" s="2" t="s">
+      <c r="J91" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT91" s="2" t="str">
@@ -14720,13 +14720,13 @@
       <c r="C92" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D92" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E92" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F92" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G92" s="2" t="n">
@@ -14735,7 +14735,7 @@
       <c r="I92" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J92" s="2" t="s">
+      <c r="J92" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT92" s="2" t="str">
@@ -14853,13 +14853,13 @@
       <c r="C93" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D93" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E93" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F93" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G93" s="2" t="n">
@@ -14868,7 +14868,7 @@
       <c r="I93" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J93" s="2" t="s">
+      <c r="J93" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT93" s="2" t="str">
@@ -14986,13 +14986,13 @@
       <c r="C94" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D94" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E94" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="F94" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G94" s="2" t="n">
@@ -15001,7 +15001,7 @@
       <c r="I94" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J94" s="2" t="s">
+      <c r="J94" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT94" s="2" t="str">
@@ -15119,13 +15119,13 @@
       <c r="C95" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E95" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G95" s="2" t="n">
@@ -15134,7 +15134,7 @@
       <c r="I95" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J95" s="2" t="s">
+      <c r="J95" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT95" s="2" t="str">
@@ -15252,13 +15252,13 @@
       <c r="C96" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E96" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F96" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G96" s="2" t="n">
@@ -15267,7 +15267,7 @@
       <c r="I96" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="J96" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT96" s="2" t="str">
@@ -15385,13 +15385,13 @@
       <c r="C97" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E97" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F97" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G97" s="2" t="n">
@@ -15400,7 +15400,7 @@
       <c r="I97" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J97" s="2" t="s">
+      <c r="J97" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT97" s="2" t="str">
@@ -15518,13 +15518,13 @@
       <c r="C98" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D98" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E98" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G98" s="2" t="n">
@@ -15533,7 +15533,7 @@
       <c r="I98" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J98" s="2" t="s">
+      <c r="J98" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT98" s="2" t="str">
@@ -15651,13 +15651,13 @@
       <c r="C99" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E99" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G99" s="2" t="n">
@@ -15666,7 +15666,7 @@
       <c r="I99" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J99" s="2" t="s">
+      <c r="J99" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT99" s="2" t="str">
@@ -15784,13 +15784,13 @@
       <c r="C100" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E100" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G100" s="2" t="n">
@@ -15799,7 +15799,7 @@
       <c r="I100" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J100" s="2" t="s">
+      <c r="J100" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT100" s="2" t="str">
@@ -15917,13 +15917,13 @@
       <c r="C101" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E101" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G101" s="2" t="n">
@@ -15932,7 +15932,7 @@
       <c r="I101" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J101" s="2" t="s">
+      <c r="J101" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT101" s="2" t="str">
@@ -16050,13 +16050,13 @@
       <c r="C102" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E102" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G102" s="2" t="n">
@@ -16065,7 +16065,7 @@
       <c r="I102" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J102" s="2" t="s">
+      <c r="J102" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT102" s="2" t="str">
@@ -16183,13 +16183,13 @@
       <c r="C103" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D103" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E103" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F103" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G103" s="2" t="n">
@@ -16198,7 +16198,7 @@
       <c r="I103" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J103" s="2" t="s">
+      <c r="J103" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT103" s="2" t="str">
@@ -16316,13 +16316,13 @@
       <c r="C104" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E104" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="F104" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G104" s="2" t="n">
@@ -16331,7 +16331,7 @@
       <c r="I104" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J104" s="2" t="s">
+      <c r="J104" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT104" s="2" t="str">
@@ -16449,13 +16449,13 @@
       <c r="C105" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E105" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="F105" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G105" s="2" t="n">
@@ -16464,7 +16464,7 @@
       <c r="I105" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J105" s="2" t="s">
+      <c r="J105" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT105" s="2" t="str">
@@ -16582,13 +16582,13 @@
       <c r="C106" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E106" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="F106" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G106" s="2" t="n">
@@ -16597,7 +16597,7 @@
       <c r="I106" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J106" s="2" t="s">
+      <c r="J106" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT106" s="2" t="str">
@@ -16715,13 +16715,13 @@
       <c r="C107" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E107" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F107" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G107" s="2" t="n">
@@ -16730,7 +16730,7 @@
       <c r="I107" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J107" s="2" t="s">
+      <c r="J107" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT107" s="2" t="str">
@@ -16848,13 +16848,13 @@
       <c r="C108" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E108" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F108" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G108" s="2" t="n">
@@ -16863,7 +16863,7 @@
       <c r="I108" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J108" s="2" t="s">
+      <c r="J108" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT108" s="2" t="str">
@@ -16981,13 +16981,13 @@
       <c r="C109" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D109" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E109" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="F109" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G109" s="2" t="n">
@@ -16996,7 +16996,7 @@
       <c r="I109" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J109" s="2" t="s">
+      <c r="J109" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT109" s="2" t="str">
@@ -17114,13 +17114,13 @@
       <c r="C110" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D110" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E110" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F110" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G110" s="2" t="n">
@@ -17129,7 +17129,7 @@
       <c r="I110" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="J110" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT110" s="2" t="str">
@@ -17247,13 +17247,13 @@
       <c r="C111" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D111" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E111" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F111" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G111" s="2" t="n">
@@ -17262,7 +17262,7 @@
       <c r="I111" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J111" s="2" t="s">
+      <c r="J111" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT111" s="2" t="str">
@@ -17380,13 +17380,13 @@
       <c r="C112" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D112" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E112" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F112" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G112" s="2" t="n">
@@ -17395,7 +17395,7 @@
       <c r="I112" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J112" s="2" t="s">
+      <c r="J112" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT112" s="2" t="str">
@@ -17513,13 +17513,13 @@
       <c r="C113" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D113" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E113" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F113" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G113" s="2" t="n">
@@ -17528,7 +17528,7 @@
       <c r="I113" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J113" s="2" t="s">
+      <c r="J113" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT113" s="2" t="str">
@@ -17646,13 +17646,13 @@
       <c r="C114" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E114" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F114" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G114" s="2" t="n">
@@ -17661,7 +17661,7 @@
       <c r="I114" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J114" s="2" t="s">
+      <c r="J114" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT114" s="2" t="str">
@@ -17779,13 +17779,13 @@
       <c r="C115" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E115" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F115" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G115" s="2" t="n">
@@ -17794,7 +17794,7 @@
       <c r="I115" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J115" s="2" t="s">
+      <c r="J115" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT115" s="2" t="str">
@@ -17912,13 +17912,13 @@
       <c r="C116" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E116" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F116" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G116" s="2" t="n">
@@ -17927,7 +17927,7 @@
       <c r="I116" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J116" s="2" t="s">
+      <c r="J116" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT116" s="2" t="str">
@@ -18045,13 +18045,13 @@
       <c r="C117" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D117" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E117" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F117" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G117" s="2" t="n">
@@ -18060,7 +18060,7 @@
       <c r="I117" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="J117" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT117" s="2" t="str">
@@ -18178,13 +18178,13 @@
       <c r="C118" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E118" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F118" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G118" s="2" t="n">
@@ -18193,7 +18193,7 @@
       <c r="I118" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J118" s="2" t="s">
+      <c r="J118" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT118" s="2" t="str">
@@ -18311,13 +18311,13 @@
       <c r="C119" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D119" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E119" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F119" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G119" s="2" t="n">
@@ -18326,7 +18326,7 @@
       <c r="I119" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J119" s="2" t="s">
+      <c r="J119" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT119" s="2" t="str">
@@ -18444,13 +18444,13 @@
       <c r="C120" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D120" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E120" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F120" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G120" s="2" t="n">
@@ -18459,7 +18459,7 @@
       <c r="I120" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J120" s="2" t="s">
+      <c r="J120" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT120" s="2" t="str">
@@ -18577,13 +18577,13 @@
       <c r="C121" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E121" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="F121" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G121" s="2" t="n">
@@ -18592,7 +18592,7 @@
       <c r="I121" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J121" s="2" t="s">
+      <c r="J121" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT121" s="2" t="str">
@@ -18710,13 +18710,13 @@
       <c r="C122" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E122" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="F122" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G122" s="2" t="n">
@@ -18725,7 +18725,7 @@
       <c r="I122" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J122" s="2" t="s">
+      <c r="J122" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT122" s="2" t="str">
@@ -18843,13 +18843,13 @@
       <c r="C123" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E123" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F123" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G123" s="2" t="n">
@@ -18858,7 +18858,7 @@
       <c r="I123" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J123" s="2" t="s">
+      <c r="J123" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT123" s="2" t="str">
@@ -18976,13 +18976,13 @@
       <c r="C124" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E124" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F124" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G124" s="2" t="n">
@@ -18991,7 +18991,7 @@
       <c r="I124" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J124" s="2" t="s">
+      <c r="J124" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT124" s="2" t="str">
@@ -19109,13 +19109,13 @@
       <c r="C125" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="D125" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E125" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F125" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G125" s="2" t="n">
@@ -19124,7 +19124,7 @@
       <c r="I125" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="J125" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT125" s="2" t="str">
@@ -19242,13 +19242,13 @@
       <c r="C126" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D126" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E126" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F126" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G126" s="2" t="n">
@@ -19257,7 +19257,7 @@
       <c r="I126" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J126" s="2" t="s">
+      <c r="J126" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT126" s="2" t="str">
@@ -19375,13 +19375,13 @@
       <c r="C127" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E127" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F127" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G127" s="2" t="n">
@@ -19390,7 +19390,7 @@
       <c r="I127" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J127" s="2" t="s">
+      <c r="J127" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT127" s="2" t="str">
@@ -19508,13 +19508,13 @@
       <c r="C128" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D128" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E128" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F128" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G128" s="2" t="n">
@@ -19523,7 +19523,7 @@
       <c r="I128" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J128" s="2" t="s">
+      <c r="J128" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT128" s="2" t="str">
@@ -19641,13 +19641,13 @@
       <c r="C129" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D129" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E129" s="10" t="n">
         <v>-99</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F129" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G129" s="2" t="n">
@@ -19656,7 +19656,7 @@
       <c r="I129" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J129" s="2" t="s">
+      <c r="J129" s="10" t="s">
         <v>44</v>
       </c>
       <c r="AT129" s="2" t="str">
@@ -19773,7 +19773,7 @@
       <c r="E131" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576 C1:C1048576">
+  <conditionalFormatting sqref="C1:C1048576 I1:I1048576 J2:J129">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"purple"</formula>
     </cfRule>
@@ -19796,7 +19796,7 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="8">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C129" type="list">
       <formula1>"blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
@@ -19805,12 +19805,28 @@
       <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-inf"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G129" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3:G129" type="decimal">
       <formula1>20</formula1>
       <formula2>2000</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D129" type="list">
+      <formula1>"-,yes,no"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E129" type="list">
-      <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-99"</formula1>
+      <formula1>"-,+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-99"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F129" type="list">
+      <formula1>"-,yes,no"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2" type="decimal">
+      <formula1>20</formula1>
+      <formula2>2000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:J129" type="list">
+      <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -19831,12 +19847,12 @@
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" activeCellId="1" sqref="J2:J129 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22897,7 +22913,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="J2:J129 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27880,7 +27896,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="J2:J129 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27978,7 +27994,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="J2:J129 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
validity for Mute in spreadsheet corrected
</commit_message>
<xml_diff>
--- a/dLiveChannelList.xlsx
+++ b/dLiveChannelList.xlsx
@@ -19790,7 +19790,7 @@
       <formula>"blue"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C129" type="list">
       <formula1>"-,blue,red,yellow,green,light blue,white,purple,black"</formula1>
       <formula2>0</formula2>
@@ -19799,15 +19799,11 @@
       <formula1>"+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-inf"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D129" type="list">
-      <formula1>"-,yes,no"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:E2 E3:E129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E129" type="list">
       <formula1>"-,+10,+5,0,-5,-10,-15,-20,-25,-30,-35,-40,-45,-99"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F129" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D129 F2:F129" type="list">
       <formula1>"-,yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>